<commit_message>
Added another high level requirement
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="452" firstSheet="1" activeTab="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="201">
   <si>
     <t>Document Title</t>
   </si>
@@ -721,12 +721,55 @@
   <si>
     <t>The mechanism used for separation shall be capable of achieving an initial relative separation velocity between each spacecraft no greater than 1 m/s</t>
   </si>
+  <si>
+    <t>RCL2-RVM1-3-1</t>
+  </si>
+  <si>
+    <t>RCL2-RVM1-3-2</t>
+  </si>
+  <si>
+    <t>RVM2 Sub-Requirements</t>
+  </si>
+  <si>
+    <r>
+      <t>The mechanism used for separation shall not cause a rotational velocity greater than 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°/s</t>
+    </r>
+  </si>
+  <si>
+    <t>The spacecraft shall have a system to be powered for the duration of the mission lifetime</t>
+  </si>
+  <si>
+    <t>RCL-RVM2-1</t>
+  </si>
+  <si>
+    <t>RCL-RVM3</t>
+  </si>
+  <si>
+    <t>RVM3 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>The spacecraft shall carry visual aids to aid in the primary spacecraft identifying it</t>
+  </si>
+  <si>
+    <t>RCL-RVM3-1</t>
+  </si>
+  <si>
+    <t>The spacecraft shall carry components necessary for the primary spacecraft to accomplish its mission goals</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -791,14 +834,19 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="0"/>
+      <color indexed="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="10"/>
-      <color indexed="9"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -841,7 +889,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1057,13 +1105,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1159,11 +1251,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1174,6 +1276,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1183,14 +1294,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1198,47 +1303,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -1315,6 +1406,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1879,85 +1975,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="44">
         <v>41582</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="41" t="s">
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="41"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="B8" s="45"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1965,7 +2061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -1973,7 +2069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1981,7 +2077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1989,7 +2085,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1997,7 +2093,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -2005,7 +2101,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
@@ -2013,7 +2109,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
@@ -2021,7 +2117,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -2029,7 +2125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
@@ -2037,7 +2133,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -2045,7 +2141,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -2053,7 +2149,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30">
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
@@ -2061,7 +2157,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30">
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
@@ -2069,7 +2165,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
@@ -2077,7 +2173,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
@@ -2085,7 +2181,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>42</v>
       </c>
@@ -2093,7 +2189,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
@@ -2101,7 +2197,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
@@ -2109,75 +2205,75 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="6">
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
-    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2187,14 +2283,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IS318"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="7" customWidth="1"/>
     <col min="2" max="2" width="19.140625" style="7" customWidth="1"/>
@@ -2208,37 +2304,37 @@
     <col min="11" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:253">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:253" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="43" t="s">
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:253">
-      <c r="A2" s="42"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
+    <row r="2" spans="1:253" x14ac:dyDescent="0.25">
+      <c r="A2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
       <c r="E2" s="8" t="s">
         <v>55</v>
       </c>
@@ -2251,24 +2347,24 @@
       <c r="H2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="45"/>
-    </row>
-    <row r="3" spans="1:253">
-      <c r="A3" s="46" t="s">
+      <c r="I2" s="50"/>
+      <c r="J2" s="47"/>
+    </row>
+    <row r="3" spans="1:253" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-    </row>
-    <row r="4" spans="1:253" s="12" customFormat="1">
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+    </row>
+    <row r="4" spans="1:253" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
@@ -2292,7 +2388,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:253" s="16" customFormat="1">
+    <row r="5" spans="1:253" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>12</v>
       </c>
@@ -2365,7 +2461,7 @@
       <c r="IP5" s="18"/>
       <c r="IS5" s="17"/>
     </row>
-    <row r="6" spans="1:253" s="12" customFormat="1" ht="45">
+    <row r="6" spans="1:253" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
@@ -2389,7 +2485,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:253" s="12" customFormat="1" ht="30">
+    <row r="7" spans="1:253" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
@@ -2413,7 +2509,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:253">
+    <row r="8" spans="1:253" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>14</v>
       </c>
@@ -2437,7 +2533,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:253" ht="30">
+    <row r="9" spans="1:253" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>14</v>
       </c>
@@ -2461,7 +2557,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:253">
+    <row r="10" spans="1:253" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>12</v>
       </c>
@@ -2485,7 +2581,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:253">
+    <row r="11" spans="1:253" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>12</v>
       </c>
@@ -2509,7 +2605,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:253">
+    <row r="12" spans="1:253" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>12</v>
       </c>
@@ -2533,7 +2629,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:253" ht="30">
+    <row r="13" spans="1:253" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
@@ -2557,7 +2653,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:253" ht="30">
+    <row r="14" spans="1:253" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>12</v>
       </c>
@@ -2582,7 +2678,7 @@
       </c>
       <c r="V14" s="24"/>
     </row>
-    <row r="15" spans="1:253">
+    <row r="15" spans="1:253" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>12</v>
       </c>
@@ -2606,7 +2702,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:253" ht="30">
+    <row r="16" spans="1:253" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>12</v>
       </c>
@@ -2630,7 +2726,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="45">
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>12</v>
       </c>
@@ -2654,7 +2750,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30">
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>14</v>
       </c>
@@ -2678,7 +2774,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>14</v>
       </c>
@@ -2702,7 +2798,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>12</v>
       </c>
@@ -2726,7 +2822,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30">
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>12</v>
       </c>
@@ -2750,7 +2846,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>12</v>
       </c>
@@ -2774,7 +2870,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>12</v>
       </c>
@@ -2798,7 +2894,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30" customHeight="1">
+    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>14</v>
       </c>
@@ -2822,7 +2918,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>14</v>
       </c>
@@ -2846,7 +2942,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>12</v>
       </c>
@@ -2870,7 +2966,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>14</v>
       </c>
@@ -2894,7 +2990,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30">
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>14</v>
       </c>
@@ -2918,7 +3014,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="45">
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>12</v>
       </c>
@@ -2942,7 +3038,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="45">
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>12</v>
       </c>
@@ -2966,7 +3062,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30">
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>12</v>
       </c>
@@ -2990,7 +3086,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="45">
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>12</v>
       </c>
@@ -3014,7 +3110,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30">
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>12</v>
       </c>
@@ -3038,7 +3134,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="30">
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
         <v>12</v>
       </c>
@@ -3062,7 +3158,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30">
+    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
         <v>12</v>
       </c>
@@ -3086,7 +3182,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="30">
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>12</v>
       </c>
@@ -3110,21 +3206,21 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="47" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>16</v>
       </c>
@@ -3148,7 +3244,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>16</v>
       </c>
@@ -3172,7 +3268,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="30">
+    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>16</v>
       </c>
@@ -3196,7 +3292,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>16</v>
       </c>
@@ -3220,21 +3316,21 @@
         <v>145</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="47" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="47"/>
-    </row>
-    <row r="43" spans="1:10" ht="30">
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>16</v>
       </c>
@@ -3258,7 +3354,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="30">
+    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>16</v>
       </c>
@@ -3282,7 +3378,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="30">
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>16</v>
       </c>
@@ -3306,21 +3402,21 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="47" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
-    </row>
-    <row r="47" spans="1:10" ht="30">
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+    </row>
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>16</v>
       </c>
@@ -3344,21 +3440,21 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="47" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="B48" s="47"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="47"/>
-      <c r="J48" s="47"/>
-    </row>
-    <row r="49" spans="1:10" ht="45">
+      <c r="B48" s="46"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
+      <c r="J48" s="46"/>
+    </row>
+    <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>16</v>
       </c>
@@ -3382,21 +3478,21 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="47" t="s">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="47"/>
-      <c r="I50" s="47"/>
-      <c r="J50" s="47"/>
-    </row>
-    <row r="51" spans="1:10" ht="45">
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+    </row>
+    <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>16</v>
       </c>
@@ -3420,805 +3516,805 @@
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C52" s="34"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C53" s="34"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C54" s="34"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C55" s="34"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C56" s="34"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C57" s="34"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C58" s="34"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C59" s="34"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C60" s="34"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C61" s="34"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C62" s="34"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C63" s="34"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C64" s="34"/>
     </row>
-    <row r="65" spans="3:3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="34"/>
     </row>
-    <row r="66" spans="3:3">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" s="34"/>
     </row>
-    <row r="67" spans="3:3">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="34"/>
     </row>
-    <row r="68" spans="3:3">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" s="34"/>
     </row>
-    <row r="69" spans="3:3">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="34"/>
     </row>
-    <row r="70" spans="3:3">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" s="34"/>
     </row>
-    <row r="71" spans="3:3">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="34"/>
     </row>
-    <row r="72" spans="3:3">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" s="34"/>
     </row>
-    <row r="73" spans="3:3">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="34"/>
     </row>
-    <row r="74" spans="3:3">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" s="34"/>
     </row>
-    <row r="75" spans="3:3">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="34"/>
     </row>
-    <row r="76" spans="3:3">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" s="34"/>
     </row>
-    <row r="77" spans="3:3">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="34"/>
     </row>
-    <row r="78" spans="3:3">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" s="34"/>
     </row>
-    <row r="79" spans="3:3">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="34"/>
     </row>
-    <row r="80" spans="3:3">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" s="34"/>
     </row>
-    <row r="81" spans="3:3">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="34"/>
     </row>
-    <row r="82" spans="3:3">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="34"/>
     </row>
-    <row r="83" spans="3:3">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="34"/>
     </row>
-    <row r="84" spans="3:3">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" s="34"/>
     </row>
-    <row r="85" spans="3:3">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="34"/>
     </row>
-    <row r="86" spans="3:3">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" s="34"/>
     </row>
-    <row r="87" spans="3:3">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="34"/>
     </row>
-    <row r="88" spans="3:3">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" s="34"/>
     </row>
-    <row r="89" spans="3:3">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="34"/>
     </row>
-    <row r="90" spans="3:3">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" s="34"/>
     </row>
-    <row r="91" spans="3:3">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="34"/>
     </row>
-    <row r="92" spans="3:3">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="34"/>
     </row>
-    <row r="93" spans="3:3">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="34"/>
     </row>
-    <row r="94" spans="3:3">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" s="34"/>
     </row>
-    <row r="95" spans="3:3">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="34"/>
     </row>
-    <row r="96" spans="3:3">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="34"/>
     </row>
-    <row r="97" spans="3:3">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="34"/>
     </row>
-    <row r="98" spans="3:3">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="34"/>
     </row>
-    <row r="99" spans="3:3">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="34"/>
     </row>
-    <row r="100" spans="3:3">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="34"/>
     </row>
-    <row r="101" spans="3:3">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="34"/>
     </row>
-    <row r="102" spans="3:3">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C102" s="34"/>
     </row>
-    <row r="103" spans="3:3">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="34"/>
     </row>
-    <row r="104" spans="3:3">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C104" s="34"/>
     </row>
-    <row r="105" spans="3:3">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="34"/>
     </row>
-    <row r="106" spans="3:3">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C106" s="34"/>
     </row>
-    <row r="107" spans="3:3">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="34"/>
     </row>
-    <row r="108" spans="3:3">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C108" s="34"/>
     </row>
-    <row r="109" spans="3:3">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C109" s="34"/>
     </row>
-    <row r="110" spans="3:3">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C110" s="34"/>
     </row>
-    <row r="111" spans="3:3">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C111" s="34"/>
     </row>
-    <row r="112" spans="3:3">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C112" s="34"/>
     </row>
-    <row r="113" spans="3:3">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C113" s="34"/>
     </row>
-    <row r="114" spans="3:3">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C114" s="34"/>
     </row>
-    <row r="115" spans="3:3">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C115" s="34"/>
     </row>
-    <row r="116" spans="3:3">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C116" s="34"/>
     </row>
-    <row r="117" spans="3:3">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C117" s="34"/>
     </row>
-    <row r="118" spans="3:3">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C118" s="34"/>
     </row>
-    <row r="119" spans="3:3">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C119" s="34"/>
     </row>
-    <row r="120" spans="3:3">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C120" s="34"/>
     </row>
-    <row r="121" spans="3:3">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C121" s="34"/>
     </row>
-    <row r="122" spans="3:3">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C122" s="34"/>
     </row>
-    <row r="123" spans="3:3">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C123" s="34"/>
     </row>
-    <row r="124" spans="3:3">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C124" s="34"/>
     </row>
-    <row r="125" spans="3:3">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C125" s="34"/>
     </row>
-    <row r="126" spans="3:3">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C126" s="34"/>
     </row>
-    <row r="127" spans="3:3">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C127" s="34"/>
     </row>
-    <row r="128" spans="3:3">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C128" s="34"/>
     </row>
-    <row r="129" spans="3:3">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="34"/>
     </row>
-    <row r="130" spans="3:3">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C130" s="34"/>
     </row>
-    <row r="131" spans="3:3">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="34"/>
     </row>
-    <row r="132" spans="3:3">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C132" s="34"/>
     </row>
-    <row r="133" spans="3:3">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="34"/>
     </row>
-    <row r="134" spans="3:3">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C134" s="34"/>
     </row>
-    <row r="135" spans="3:3">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="34"/>
     </row>
-    <row r="136" spans="3:3">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C136" s="34"/>
     </row>
-    <row r="137" spans="3:3">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="34"/>
     </row>
-    <row r="138" spans="3:3">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C138" s="34"/>
     </row>
-    <row r="139" spans="3:3">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="34"/>
     </row>
-    <row r="140" spans="3:3">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C140" s="34"/>
     </row>
-    <row r="141" spans="3:3">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="34"/>
     </row>
-    <row r="142" spans="3:3">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C142" s="34"/>
     </row>
-    <row r="143" spans="3:3">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="34"/>
     </row>
-    <row r="144" spans="3:3">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C144" s="34"/>
     </row>
-    <row r="145" spans="3:3">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="34"/>
     </row>
-    <row r="146" spans="3:3">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C146" s="34"/>
     </row>
-    <row r="147" spans="3:3">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C147" s="34"/>
     </row>
-    <row r="148" spans="3:3">
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C148" s="34"/>
     </row>
-    <row r="149" spans="3:3">
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C149" s="34"/>
     </row>
-    <row r="150" spans="3:3">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C150" s="34"/>
     </row>
-    <row r="151" spans="3:3">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C151" s="34"/>
     </row>
-    <row r="152" spans="3:3">
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C152" s="34"/>
     </row>
-    <row r="153" spans="3:3">
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C153" s="34"/>
     </row>
-    <row r="154" spans="3:3">
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C154" s="34"/>
     </row>
-    <row r="155" spans="3:3">
+    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C155" s="34"/>
     </row>
-    <row r="156" spans="3:3">
+    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C156" s="34"/>
     </row>
-    <row r="157" spans="3:3">
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C157" s="34"/>
     </row>
-    <row r="158" spans="3:3">
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C158" s="34"/>
     </row>
-    <row r="159" spans="3:3">
+    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C159" s="34"/>
     </row>
-    <row r="160" spans="3:3">
+    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C160" s="34"/>
     </row>
-    <row r="161" spans="3:3">
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C161" s="34"/>
     </row>
-    <row r="162" spans="3:3">
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C162" s="34"/>
     </row>
-    <row r="163" spans="3:3">
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C163" s="34"/>
     </row>
-    <row r="164" spans="3:3">
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C164" s="34"/>
     </row>
-    <row r="165" spans="3:3">
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C165" s="34"/>
     </row>
-    <row r="166" spans="3:3">
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C166" s="34"/>
     </row>
-    <row r="167" spans="3:3">
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C167" s="34"/>
     </row>
-    <row r="168" spans="3:3">
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C168" s="34"/>
     </row>
-    <row r="169" spans="3:3">
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C169" s="34"/>
     </row>
-    <row r="170" spans="3:3">
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C170" s="34"/>
     </row>
-    <row r="171" spans="3:3">
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C171" s="34"/>
     </row>
-    <row r="172" spans="3:3">
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C172" s="34"/>
     </row>
-    <row r="173" spans="3:3">
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C173" s="34"/>
     </row>
-    <row r="174" spans="3:3">
+    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C174" s="34"/>
     </row>
-    <row r="175" spans="3:3">
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C175" s="34"/>
     </row>
-    <row r="176" spans="3:3">
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C176" s="34"/>
     </row>
-    <row r="177" spans="3:3">
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C177" s="34"/>
     </row>
-    <row r="178" spans="3:3">
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C178" s="34"/>
     </row>
-    <row r="179" spans="3:3">
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C179" s="34"/>
     </row>
-    <row r="180" spans="3:3">
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C180" s="34"/>
     </row>
-    <row r="181" spans="3:3">
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C181" s="34"/>
     </row>
-    <row r="182" spans="3:3">
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C182" s="34"/>
     </row>
-    <row r="183" spans="3:3">
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C183" s="34"/>
     </row>
-    <row r="184" spans="3:3">
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C184" s="34"/>
     </row>
-    <row r="185" spans="3:3">
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C185" s="34"/>
     </row>
-    <row r="186" spans="3:3">
+    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C186" s="34"/>
     </row>
-    <row r="187" spans="3:3">
+    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C187" s="34"/>
     </row>
-    <row r="188" spans="3:3">
+    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C188" s="34"/>
     </row>
-    <row r="189" spans="3:3">
+    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C189" s="34"/>
     </row>
-    <row r="190" spans="3:3">
+    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C190" s="34"/>
     </row>
-    <row r="191" spans="3:3">
+    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C191" s="34"/>
     </row>
-    <row r="192" spans="3:3">
+    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C192" s="34"/>
     </row>
-    <row r="193" spans="3:3">
+    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C193" s="34"/>
     </row>
-    <row r="194" spans="3:3">
+    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C194" s="34"/>
     </row>
-    <row r="195" spans="3:3">
+    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C195" s="34"/>
     </row>
-    <row r="196" spans="3:3">
+    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C196" s="34"/>
     </row>
-    <row r="197" spans="3:3">
+    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C197" s="34"/>
     </row>
-    <row r="198" spans="3:3">
+    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C198" s="34"/>
     </row>
-    <row r="199" spans="3:3">
+    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C199" s="34"/>
     </row>
-    <row r="200" spans="3:3">
+    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C200" s="34"/>
     </row>
-    <row r="201" spans="3:3">
+    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C201" s="34"/>
     </row>
-    <row r="202" spans="3:3">
+    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C202" s="34"/>
     </row>
-    <row r="203" spans="3:3">
+    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C203" s="34"/>
     </row>
-    <row r="204" spans="3:3">
+    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C204" s="34"/>
     </row>
-    <row r="205" spans="3:3">
+    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C205" s="34"/>
     </row>
-    <row r="206" spans="3:3">
+    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C206" s="34"/>
     </row>
-    <row r="207" spans="3:3">
+    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C207" s="34"/>
     </row>
-    <row r="208" spans="3:3">
+    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C208" s="34"/>
     </row>
-    <row r="209" spans="3:3">
+    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C209" s="34"/>
     </row>
-    <row r="210" spans="3:3">
+    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C210" s="34"/>
     </row>
-    <row r="211" spans="3:3">
+    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C211" s="34"/>
     </row>
-    <row r="212" spans="3:3">
+    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C212" s="34"/>
     </row>
-    <row r="213" spans="3:3">
+    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C213" s="34"/>
     </row>
-    <row r="214" spans="3:3">
+    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C214" s="34"/>
     </row>
-    <row r="215" spans="3:3">
+    <row r="215" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C215" s="34"/>
     </row>
-    <row r="216" spans="3:3">
+    <row r="216" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C216" s="34"/>
     </row>
-    <row r="217" spans="3:3">
+    <row r="217" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C217" s="34"/>
     </row>
-    <row r="218" spans="3:3">
+    <row r="218" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C218" s="34"/>
     </row>
-    <row r="219" spans="3:3">
+    <row r="219" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C219" s="34"/>
     </row>
-    <row r="220" spans="3:3">
+    <row r="220" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C220" s="34"/>
     </row>
-    <row r="221" spans="3:3">
+    <row r="221" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C221" s="34"/>
     </row>
-    <row r="222" spans="3:3">
+    <row r="222" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C222" s="34"/>
     </row>
-    <row r="223" spans="3:3">
+    <row r="223" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C223" s="34"/>
     </row>
-    <row r="224" spans="3:3">
+    <row r="224" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C224" s="34"/>
     </row>
-    <row r="225" spans="3:3">
+    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C225" s="34"/>
     </row>
-    <row r="226" spans="3:3">
+    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C226" s="34"/>
     </row>
-    <row r="227" spans="3:3">
+    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C227" s="34"/>
     </row>
-    <row r="228" spans="3:3">
+    <row r="228" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C228" s="34"/>
     </row>
-    <row r="229" spans="3:3">
+    <row r="229" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C229" s="34"/>
     </row>
-    <row r="230" spans="3:3">
+    <row r="230" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C230" s="34"/>
     </row>
-    <row r="231" spans="3:3">
+    <row r="231" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C231" s="34"/>
     </row>
-    <row r="232" spans="3:3">
+    <row r="232" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C232" s="34"/>
     </row>
-    <row r="233" spans="3:3">
+    <row r="233" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C233" s="34"/>
     </row>
-    <row r="234" spans="3:3">
+    <row r="234" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C234" s="34"/>
     </row>
-    <row r="235" spans="3:3">
+    <row r="235" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C235" s="34"/>
     </row>
-    <row r="236" spans="3:3">
+    <row r="236" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C236" s="34"/>
     </row>
-    <row r="237" spans="3:3">
+    <row r="237" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C237" s="34"/>
     </row>
-    <row r="238" spans="3:3">
+    <row r="238" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C238" s="34"/>
     </row>
-    <row r="239" spans="3:3">
+    <row r="239" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C239" s="34"/>
     </row>
-    <row r="240" spans="3:3">
+    <row r="240" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C240" s="34"/>
     </row>
-    <row r="241" spans="3:3">
+    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C241" s="34"/>
     </row>
-    <row r="242" spans="3:3">
+    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C242" s="34"/>
     </row>
-    <row r="243" spans="3:3">
+    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C243" s="34"/>
     </row>
-    <row r="244" spans="3:3">
+    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C244" s="34"/>
     </row>
-    <row r="245" spans="3:3">
+    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C245" s="34"/>
     </row>
-    <row r="246" spans="3:3">
+    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C246" s="34"/>
     </row>
-    <row r="247" spans="3:3">
+    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C247" s="34"/>
     </row>
-    <row r="248" spans="3:3">
+    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C248" s="34"/>
     </row>
-    <row r="249" spans="3:3">
+    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C249" s="34"/>
     </row>
-    <row r="250" spans="3:3">
+    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C250" s="34"/>
     </row>
-    <row r="251" spans="3:3">
+    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C251" s="34"/>
     </row>
-    <row r="252" spans="3:3">
+    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C252" s="34"/>
     </row>
-    <row r="253" spans="3:3">
+    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C253" s="34"/>
     </row>
-    <row r="254" spans="3:3">
+    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C254" s="34"/>
     </row>
-    <row r="255" spans="3:3">
+    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C255" s="34"/>
     </row>
-    <row r="256" spans="3:3">
+    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C256" s="34"/>
     </row>
-    <row r="257" spans="3:3">
+    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C257" s="34"/>
     </row>
-    <row r="258" spans="3:3">
+    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C258" s="34"/>
     </row>
-    <row r="259" spans="3:3">
+    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C259" s="34"/>
     </row>
-    <row r="260" spans="3:3">
+    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C260" s="34"/>
     </row>
-    <row r="261" spans="3:3">
+    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C261" s="34"/>
     </row>
-    <row r="262" spans="3:3">
+    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C262" s="34"/>
     </row>
-    <row r="263" spans="3:3">
+    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C263" s="34"/>
     </row>
-    <row r="264" spans="3:3">
+    <row r="264" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C264" s="34"/>
     </row>
-    <row r="265" spans="3:3">
+    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C265" s="34"/>
     </row>
-    <row r="266" spans="3:3">
+    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C266" s="34"/>
     </row>
-    <row r="267" spans="3:3">
+    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C267" s="34"/>
     </row>
-    <row r="268" spans="3:3">
+    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C268" s="34"/>
     </row>
-    <row r="269" spans="3:3">
+    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C269" s="34"/>
     </row>
-    <row r="270" spans="3:3">
+    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C270" s="34"/>
     </row>
-    <row r="271" spans="3:3">
+    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C271" s="34"/>
     </row>
-    <row r="272" spans="3:3">
+    <row r="272" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C272" s="34"/>
     </row>
-    <row r="273" spans="3:3">
+    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C273" s="34"/>
     </row>
-    <row r="274" spans="3:3">
+    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C274" s="34"/>
     </row>
-    <row r="275" spans="3:3">
+    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C275" s="34"/>
     </row>
-    <row r="276" spans="3:3">
+    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C276" s="34"/>
     </row>
-    <row r="277" spans="3:3">
+    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C277" s="34"/>
     </row>
-    <row r="278" spans="3:3">
+    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C278" s="34"/>
     </row>
-    <row r="279" spans="3:3">
+    <row r="279" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C279" s="34"/>
     </row>
-    <row r="280" spans="3:3">
+    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C280" s="34"/>
     </row>
-    <row r="281" spans="3:3">
+    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C281" s="34"/>
     </row>
-    <row r="282" spans="3:3">
+    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C282" s="34"/>
     </row>
-    <row r="283" spans="3:3">
+    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C283" s="34"/>
     </row>
-    <row r="284" spans="3:3">
+    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C284" s="34"/>
     </row>
-    <row r="285" spans="3:3">
+    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C285" s="34"/>
     </row>
-    <row r="286" spans="3:3">
+    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C286" s="34"/>
     </row>
-    <row r="287" spans="3:3">
+    <row r="287" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C287" s="34"/>
     </row>
-    <row r="288" spans="3:3">
+    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C288" s="34"/>
     </row>
-    <row r="289" spans="3:3">
+    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C289" s="34"/>
     </row>
-    <row r="290" spans="3:3">
+    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C290" s="34"/>
     </row>
-    <row r="291" spans="3:3">
+    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C291" s="34"/>
     </row>
-    <row r="292" spans="3:3">
+    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C292" s="34"/>
     </row>
-    <row r="293" spans="3:3">
+    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C293" s="34"/>
     </row>
-    <row r="294" spans="3:3">
+    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C294" s="34"/>
     </row>
-    <row r="295" spans="3:3">
+    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C295" s="34"/>
     </row>
-    <row r="296" spans="3:3">
+    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C296" s="34"/>
     </row>
-    <row r="297" spans="3:3">
+    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C297" s="34"/>
     </row>
-    <row r="298" spans="3:3">
+    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C298" s="34"/>
     </row>
-    <row r="299" spans="3:3">
+    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C299" s="34"/>
     </row>
-    <row r="300" spans="3:3">
+    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C300" s="34"/>
     </row>
-    <row r="301" spans="3:3">
+    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C301" s="34"/>
     </row>
-    <row r="302" spans="3:3">
+    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C302" s="34"/>
     </row>
-    <row r="303" spans="3:3">
+    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C303" s="34"/>
     </row>
-    <row r="304" spans="3:3">
+    <row r="304" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C304" s="34"/>
     </row>
-    <row r="305" spans="3:3">
+    <row r="305" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C305" s="34"/>
     </row>
-    <row r="306" spans="3:3">
+    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C306" s="34"/>
     </row>
-    <row r="307" spans="3:3">
+    <row r="307" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C307" s="34"/>
     </row>
-    <row r="308" spans="3:3">
+    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C308" s="34"/>
     </row>
-    <row r="309" spans="3:3">
+    <row r="309" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C309" s="34"/>
     </row>
-    <row r="310" spans="3:3">
+    <row r="310" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C310" s="34"/>
     </row>
-    <row r="311" spans="3:3">
+    <row r="311" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C311" s="34"/>
     </row>
-    <row r="312" spans="3:3">
+    <row r="312" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C312" s="34"/>
     </row>
-    <row r="313" spans="3:3">
+    <row r="313" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C313" s="34"/>
     </row>
-    <row r="314" spans="3:3">
+    <row r="314" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C314" s="34"/>
     </row>
-    <row r="315" spans="3:3">
+    <row r="315" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C315" s="34"/>
     </row>
-    <row r="316" spans="3:3">
+    <row r="316" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C316" s="34"/>
     </row>
-    <row r="317" spans="3:3">
+    <row r="317" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C317" s="34"/>
     </row>
-    <row r="318" spans="3:3">
+    <row r="318" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C318" s="34"/>
     </row>
   </sheetData>
@@ -4245,14 +4341,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G194"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T195"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:G14"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60.28515625" style="35" customWidth="1"/>
     <col min="2" max="5" width="9.140625" style="36"/>
@@ -4261,25 +4357,25 @@
     <col min="8" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.25">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="43" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="47" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25">
-      <c r="A2" s="43"/>
+    <row r="2" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="50"/>
       <c r="B2" s="8" t="s">
         <v>55</v>
       </c>
@@ -4292,751 +4388,1525 @@
       <c r="E2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="45"/>
-    </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A3" s="58" t="s">
+      <c r="F2" s="50"/>
+      <c r="G2" s="47"/>
+    </row>
+    <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-    </row>
-    <row r="4" spans="1:7" ht="30">
-      <c r="A4" s="38" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+    </row>
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="63" t="s">
         <v>174</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="37" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="40" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
-      <c r="A5" s="59" t="s">
+    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="B5" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60" t="s">
+      <c r="B5" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="38" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="56" t="s">
+    <row r="6" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-    </row>
-    <row r="7" spans="1:7" ht="30">
-      <c r="A7" s="52" t="s">
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+    </row>
+    <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="51" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="G8" s="38" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30">
-      <c r="A8" s="52" t="s">
+    <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="B8" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="53"/>
-      <c r="F8" s="51" t="s">
+      <c r="B9" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G9" s="38" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="52" t="s">
+    <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="51" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="G10" s="38" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="54" t="s">
+    <row r="11" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-    </row>
-    <row r="11" spans="1:7" s="62" customFormat="1" ht="30">
-      <c r="A11" s="52" t="s">
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+    </row>
+    <row r="12" spans="1:20" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="B11" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51" t="s">
+      <c r="B12" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G12" s="38" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="62" customFormat="1" ht="30">
-      <c r="A12" s="50" t="s">
+    <row r="13" spans="1:20" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="B12" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51" t="s">
+      <c r="B13" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="G12" s="51" t="s">
+      <c r="G13" s="38" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="62" customFormat="1" ht="15">
-      <c r="A13" s="54" t="s">
+    <row r="14" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="59" t="s">
         <v>188</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-    </row>
-    <row r="14" spans="1:7" s="62" customFormat="1" ht="45">
-      <c r="A14" s="50" t="s">
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+    </row>
+    <row r="15" spans="1:20" s="41" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-    </row>
-    <row r="15" spans="1:7" s="62" customFormat="1" ht="15">
-      <c r="A15" s="63"/>
-    </row>
-    <row r="16" spans="1:7" s="62" customFormat="1" ht="15">
-      <c r="A16" s="63"/>
-    </row>
-    <row r="17" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A17" s="63"/>
-    </row>
-    <row r="18" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A18" s="63"/>
-    </row>
-    <row r="19" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A19" s="63"/>
-    </row>
-    <row r="20" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A20" s="63"/>
-    </row>
-    <row r="21" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A21" s="63"/>
-    </row>
-    <row r="22" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A22" s="63"/>
-    </row>
-    <row r="23" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A23" s="63"/>
-    </row>
-    <row r="24" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A24" s="63"/>
-    </row>
-    <row r="25" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A25" s="63"/>
-    </row>
-    <row r="26" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A26" s="63"/>
-    </row>
-    <row r="27" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A27" s="63"/>
-    </row>
-    <row r="28" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A28" s="63"/>
-    </row>
-    <row r="29" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A29" s="63"/>
-    </row>
-    <row r="30" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A30" s="63"/>
-    </row>
-    <row r="31" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A31" s="63"/>
-    </row>
-    <row r="32" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A32" s="63"/>
-    </row>
-    <row r="33" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A33" s="63"/>
-    </row>
-    <row r="34" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A34" s="63"/>
-    </row>
-    <row r="35" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A35" s="63"/>
-    </row>
-    <row r="36" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A36" s="63"/>
-    </row>
-    <row r="37" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A37" s="63"/>
-    </row>
-    <row r="38" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A38" s="63"/>
-    </row>
-    <row r="39" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A39" s="63"/>
-    </row>
-    <row r="40" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A40" s="63"/>
-    </row>
-    <row r="41" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A41" s="63"/>
-    </row>
-    <row r="42" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A42" s="63"/>
-    </row>
-    <row r="43" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A43" s="63"/>
-    </row>
-    <row r="44" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A44" s="63"/>
-    </row>
-    <row r="45" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A45" s="63"/>
-    </row>
-    <row r="46" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A46" s="63"/>
-    </row>
-    <row r="47" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A47" s="63"/>
-    </row>
-    <row r="48" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A48" s="63"/>
-    </row>
-    <row r="49" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A49" s="63"/>
-    </row>
-    <row r="50" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A50" s="63"/>
-    </row>
-    <row r="51" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A51" s="63"/>
-    </row>
-    <row r="52" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A52" s="63"/>
-    </row>
-    <row r="53" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A53" s="63"/>
-    </row>
-    <row r="54" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A54" s="63"/>
-    </row>
-    <row r="55" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A55" s="63"/>
-    </row>
-    <row r="56" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A56" s="63"/>
-    </row>
-    <row r="57" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A57" s="63"/>
-    </row>
-    <row r="58" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A58" s="63"/>
-    </row>
-    <row r="59" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A59" s="63"/>
-    </row>
-    <row r="60" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A60" s="63"/>
-    </row>
-    <row r="61" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A61" s="63"/>
-    </row>
-    <row r="62" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A62" s="63"/>
-    </row>
-    <row r="63" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A63" s="63"/>
-    </row>
-    <row r="64" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A64" s="63"/>
-    </row>
-    <row r="65" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A65" s="63"/>
-    </row>
-    <row r="66" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A66" s="63"/>
-    </row>
-    <row r="67" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A67" s="63"/>
-    </row>
-    <row r="68" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A68" s="63"/>
-    </row>
-    <row r="69" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A69" s="63"/>
-    </row>
-    <row r="70" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A70" s="63"/>
-    </row>
-    <row r="71" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A71" s="63"/>
-    </row>
-    <row r="72" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A72" s="63"/>
-    </row>
-    <row r="73" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A73" s="63"/>
-    </row>
-    <row r="74" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A74" s="63"/>
-    </row>
-    <row r="75" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A75" s="63"/>
-    </row>
-    <row r="76" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A76" s="63"/>
-    </row>
-    <row r="77" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A77" s="63"/>
-    </row>
-    <row r="78" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A78" s="63"/>
-    </row>
-    <row r="79" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A79" s="63"/>
-    </row>
-    <row r="80" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A80" s="63"/>
-    </row>
-    <row r="81" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A81" s="63"/>
-    </row>
-    <row r="82" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A82" s="63"/>
-    </row>
-    <row r="83" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A83" s="63"/>
-    </row>
-    <row r="84" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A84" s="63"/>
-    </row>
-    <row r="85" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A85" s="63"/>
-    </row>
-    <row r="86" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A86" s="63"/>
-    </row>
-    <row r="87" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A87" s="63"/>
-    </row>
-    <row r="88" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A88" s="63"/>
-    </row>
-    <row r="89" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A89" s="63"/>
-    </row>
-    <row r="90" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A90" s="63"/>
-    </row>
-    <row r="91" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A91" s="63"/>
-    </row>
-    <row r="92" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A92" s="63"/>
-    </row>
-    <row r="93" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A93" s="63"/>
-    </row>
-    <row r="94" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A94" s="63"/>
-    </row>
-    <row r="95" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A95" s="63"/>
-    </row>
-    <row r="96" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A96" s="63"/>
-    </row>
-    <row r="97" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A97" s="63"/>
-    </row>
-    <row r="98" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A98" s="63"/>
-    </row>
-    <row r="99" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A99" s="63"/>
-    </row>
-    <row r="100" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A100" s="63"/>
-    </row>
-    <row r="101" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A101" s="63"/>
-    </row>
-    <row r="102" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A102" s="63"/>
-    </row>
-    <row r="103" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A103" s="63"/>
-    </row>
-    <row r="104" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A104" s="63"/>
-    </row>
-    <row r="105" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A105" s="63"/>
-    </row>
-    <row r="106" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A106" s="63"/>
-    </row>
-    <row r="107" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A107" s="63"/>
-    </row>
-    <row r="108" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A108" s="63"/>
-    </row>
-    <row r="109" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A109" s="63"/>
-    </row>
-    <row r="110" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A110" s="63"/>
-    </row>
-    <row r="111" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A111" s="63"/>
-    </row>
-    <row r="112" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A112" s="63"/>
-    </row>
-    <row r="113" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A113" s="63"/>
-    </row>
-    <row r="114" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A114" s="63"/>
-    </row>
-    <row r="115" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A115" s="63"/>
-    </row>
-    <row r="116" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A116" s="63"/>
-    </row>
-    <row r="117" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A117" s="63"/>
-    </row>
-    <row r="118" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A118" s="63"/>
-    </row>
-    <row r="119" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A119" s="63"/>
-    </row>
-    <row r="120" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A120" s="63"/>
-    </row>
-    <row r="121" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A121" s="63"/>
-    </row>
-    <row r="122" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A122" s="63"/>
-    </row>
-    <row r="123" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A123" s="63"/>
-    </row>
-    <row r="124" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A124" s="63"/>
-    </row>
-    <row r="125" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A125" s="63"/>
-    </row>
-    <row r="126" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A126" s="63"/>
-    </row>
-    <row r="127" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A127" s="63"/>
-    </row>
-    <row r="128" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A128" s="63"/>
-    </row>
-    <row r="129" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A129" s="63"/>
-    </row>
-    <row r="130" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A130" s="63"/>
-    </row>
-    <row r="131" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A131" s="63"/>
-    </row>
-    <row r="132" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A132" s="63"/>
-    </row>
-    <row r="133" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A133" s="63"/>
-    </row>
-    <row r="134" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A134" s="63"/>
-    </row>
-    <row r="135" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A135" s="63"/>
-    </row>
-    <row r="136" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A136" s="63"/>
-    </row>
-    <row r="137" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A137" s="63"/>
-    </row>
-    <row r="138" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A138" s="63"/>
-    </row>
-    <row r="139" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A139" s="63"/>
-    </row>
-    <row r="140" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A140" s="63"/>
-    </row>
-    <row r="141" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A141" s="63"/>
-    </row>
-    <row r="142" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A142" s="63"/>
-    </row>
-    <row r="143" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A143" s="63"/>
-    </row>
-    <row r="144" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A144" s="63"/>
-    </row>
-    <row r="145" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A145" s="63"/>
-    </row>
-    <row r="146" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A146" s="63"/>
-    </row>
-    <row r="147" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A147" s="63"/>
-    </row>
-    <row r="148" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A148" s="63"/>
-    </row>
-    <row r="149" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A149" s="63"/>
-    </row>
-    <row r="150" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A150" s="63"/>
-    </row>
-    <row r="151" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A151" s="63"/>
-    </row>
-    <row r="152" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A152" s="63"/>
-    </row>
-    <row r="153" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A153" s="63"/>
-    </row>
-    <row r="154" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A154" s="63"/>
-    </row>
-    <row r="155" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A155" s="63"/>
-    </row>
-    <row r="156" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A156" s="63"/>
-    </row>
-    <row r="157" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A157" s="63"/>
-    </row>
-    <row r="158" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A158" s="63"/>
-    </row>
-    <row r="159" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A159" s="63"/>
-    </row>
-    <row r="160" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A160" s="63"/>
-    </row>
-    <row r="161" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A161" s="63"/>
-    </row>
-    <row r="162" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A162" s="63"/>
-    </row>
-    <row r="163" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A163" s="63"/>
-    </row>
-    <row r="164" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A164" s="63"/>
-    </row>
-    <row r="165" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A165" s="63"/>
-    </row>
-    <row r="166" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A166" s="63"/>
-    </row>
-    <row r="167" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A167" s="63"/>
-    </row>
-    <row r="168" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A168" s="63"/>
-    </row>
-    <row r="169" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A169" s="63"/>
-    </row>
-    <row r="170" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A170" s="63"/>
-    </row>
-    <row r="171" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A171" s="63"/>
-    </row>
-    <row r="172" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A172" s="63"/>
-    </row>
-    <row r="173" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A173" s="63"/>
-    </row>
-    <row r="174" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A174" s="63"/>
-    </row>
-    <row r="175" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A175" s="63"/>
-    </row>
-    <row r="176" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A176" s="63"/>
-    </row>
-    <row r="177" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A177" s="63"/>
-    </row>
-    <row r="178" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A178" s="63"/>
-    </row>
-    <row r="179" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A179" s="63"/>
-    </row>
-    <row r="180" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A180" s="63"/>
-    </row>
-    <row r="181" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A181" s="63"/>
-    </row>
-    <row r="182" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A182" s="63"/>
-    </row>
-    <row r="183" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A183" s="63"/>
-    </row>
-    <row r="184" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A184" s="63"/>
-    </row>
-    <row r="185" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A185" s="63"/>
-    </row>
-    <row r="186" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A186" s="63"/>
-    </row>
-    <row r="187" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A187" s="63"/>
-    </row>
-    <row r="188" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A188" s="63"/>
-    </row>
-    <row r="189" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A189" s="63"/>
-    </row>
-    <row r="190" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A190" s="63"/>
-    </row>
-    <row r="191" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A191" s="63"/>
-    </row>
-    <row r="192" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A192" s="63"/>
-    </row>
-    <row r="193" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A193" s="63"/>
-    </row>
-    <row r="194" spans="1:1" s="62" customFormat="1" ht="15">
-      <c r="A194" s="63"/>
+      <c r="B15" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="56"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+    </row>
+    <row r="17" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="61" t="s">
+        <v>192</v>
+      </c>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+    </row>
+    <row r="18" spans="1:20" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="56"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="56"/>
+      <c r="S18" s="56"/>
+      <c r="T18" s="56"/>
+    </row>
+    <row r="19" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="56"/>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="56"/>
+      <c r="R19" s="56"/>
+      <c r="S19" s="56"/>
+      <c r="T19" s="56"/>
+    </row>
+    <row r="20" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="56"/>
+      <c r="S20" s="56"/>
+      <c r="T20" s="56"/>
+    </row>
+    <row r="21" spans="1:20" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="56"/>
+      <c r="S21" s="56"/>
+      <c r="T21" s="56"/>
+    </row>
+    <row r="22" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="55"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="56"/>
+      <c r="S22" s="56"/>
+      <c r="T22" s="56"/>
+    </row>
+    <row r="23" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="55"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="56"/>
+      <c r="S23" s="56"/>
+      <c r="T23" s="56"/>
+    </row>
+    <row r="24" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="55"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="56"/>
+      <c r="P24" s="56"/>
+      <c r="Q24" s="56"/>
+      <c r="R24" s="56"/>
+      <c r="S24" s="56"/>
+      <c r="T24" s="56"/>
+    </row>
+    <row r="25" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="55"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="56"/>
+      <c r="Q25" s="56"/>
+      <c r="R25" s="56"/>
+      <c r="S25" s="56"/>
+      <c r="T25" s="56"/>
+    </row>
+    <row r="26" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="56"/>
+      <c r="R26" s="56"/>
+      <c r="S26" s="56"/>
+      <c r="T26" s="56"/>
+    </row>
+    <row r="27" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="55"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="56"/>
+      <c r="R27" s="56"/>
+      <c r="S27" s="56"/>
+      <c r="T27" s="56"/>
+    </row>
+    <row r="28" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="55"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="56"/>
+    </row>
+    <row r="29" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="55"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="56"/>
+    </row>
+    <row r="30" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="55"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="56"/>
+      <c r="S30" s="56"/>
+      <c r="T30" s="56"/>
+    </row>
+    <row r="31" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="55"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="56"/>
+      <c r="S31" s="56"/>
+      <c r="T31" s="56"/>
+    </row>
+    <row r="32" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="55"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="56"/>
+      <c r="S32" s="56"/>
+      <c r="T32" s="56"/>
+    </row>
+    <row r="33" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="55"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="56"/>
+      <c r="P33" s="56"/>
+      <c r="Q33" s="56"/>
+      <c r="R33" s="56"/>
+      <c r="S33" s="56"/>
+      <c r="T33" s="56"/>
+    </row>
+    <row r="34" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="55"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
+      <c r="L34" s="56"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="56"/>
+      <c r="O34" s="56"/>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="56"/>
+      <c r="R34" s="56"/>
+      <c r="S34" s="56"/>
+      <c r="T34" s="56"/>
+    </row>
+    <row r="35" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="55"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="56"/>
+      <c r="S35" s="56"/>
+      <c r="T35" s="56"/>
+    </row>
+    <row r="36" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="55"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="56"/>
+      <c r="K36" s="56"/>
+      <c r="L36" s="56"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="56"/>
+      <c r="P36" s="56"/>
+      <c r="Q36" s="56"/>
+      <c r="R36" s="56"/>
+      <c r="S36" s="56"/>
+      <c r="T36" s="56"/>
+    </row>
+    <row r="37" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="55"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="56"/>
+      <c r="O37" s="56"/>
+      <c r="P37" s="56"/>
+      <c r="Q37" s="56"/>
+      <c r="R37" s="56"/>
+      <c r="S37" s="56"/>
+      <c r="T37" s="56"/>
+    </row>
+    <row r="38" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="55"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="56"/>
+      <c r="L38" s="56"/>
+      <c r="M38" s="56"/>
+      <c r="N38" s="56"/>
+      <c r="O38" s="56"/>
+      <c r="P38" s="56"/>
+      <c r="Q38" s="56"/>
+      <c r="R38" s="56"/>
+      <c r="S38" s="56"/>
+      <c r="T38" s="56"/>
+    </row>
+    <row r="39" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="55"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
+      <c r="J39" s="56"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="56"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="56"/>
+      <c r="O39" s="56"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="56"/>
+      <c r="R39" s="56"/>
+      <c r="S39" s="56"/>
+      <c r="T39" s="56"/>
+    </row>
+    <row r="40" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="55"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="56"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="56"/>
+      <c r="L40" s="56"/>
+      <c r="M40" s="56"/>
+      <c r="N40" s="56"/>
+      <c r="O40" s="56"/>
+      <c r="P40" s="56"/>
+      <c r="Q40" s="56"/>
+      <c r="R40" s="56"/>
+      <c r="S40" s="56"/>
+      <c r="T40" s="56"/>
+    </row>
+    <row r="41" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="55"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="56"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="56"/>
+      <c r="J41" s="56"/>
+      <c r="K41" s="56"/>
+      <c r="L41" s="56"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="56"/>
+      <c r="O41" s="56"/>
+      <c r="P41" s="56"/>
+      <c r="Q41" s="56"/>
+      <c r="R41" s="56"/>
+      <c r="S41" s="56"/>
+      <c r="T41" s="56"/>
+    </row>
+    <row r="42" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="55"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="56"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="56"/>
+      <c r="L42" s="56"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
+      <c r="O42" s="56"/>
+      <c r="P42" s="56"/>
+      <c r="Q42" s="56"/>
+      <c r="R42" s="56"/>
+      <c r="S42" s="56"/>
+      <c r="T42" s="56"/>
+    </row>
+    <row r="43" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="55"/>
+      <c r="B43" s="56"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="56"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="56"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="56"/>
+      <c r="I43" s="56"/>
+      <c r="J43" s="56"/>
+      <c r="K43" s="56"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="56"/>
+      <c r="N43" s="56"/>
+      <c r="O43" s="56"/>
+      <c r="P43" s="56"/>
+      <c r="Q43" s="56"/>
+      <c r="R43" s="56"/>
+      <c r="S43" s="56"/>
+      <c r="T43" s="56"/>
+    </row>
+    <row r="44" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="55"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="56"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="56"/>
+      <c r="O44" s="56"/>
+      <c r="P44" s="56"/>
+      <c r="Q44" s="56"/>
+      <c r="R44" s="56"/>
+      <c r="S44" s="56"/>
+      <c r="T44" s="56"/>
+    </row>
+    <row r="45" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="55"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="56"/>
+      <c r="O45" s="56"/>
+      <c r="P45" s="56"/>
+      <c r="Q45" s="56"/>
+      <c r="R45" s="56"/>
+      <c r="S45" s="56"/>
+      <c r="T45" s="56"/>
+    </row>
+    <row r="46" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="55"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="56"/>
+      <c r="L46" s="56"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="56"/>
+      <c r="O46" s="56"/>
+      <c r="P46" s="56"/>
+      <c r="Q46" s="56"/>
+      <c r="R46" s="56"/>
+      <c r="S46" s="56"/>
+      <c r="T46" s="56"/>
+    </row>
+    <row r="47" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="55"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="56"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="56"/>
+      <c r="N47" s="56"/>
+      <c r="O47" s="56"/>
+      <c r="P47" s="56"/>
+      <c r="Q47" s="56"/>
+      <c r="R47" s="56"/>
+      <c r="S47" s="56"/>
+      <c r="T47" s="56"/>
+    </row>
+    <row r="48" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="55"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="56"/>
+      <c r="J48" s="56"/>
+      <c r="K48" s="56"/>
+      <c r="L48" s="56"/>
+      <c r="M48" s="56"/>
+      <c r="N48" s="56"/>
+      <c r="O48" s="56"/>
+      <c r="P48" s="56"/>
+      <c r="Q48" s="56"/>
+      <c r="R48" s="56"/>
+      <c r="S48" s="56"/>
+      <c r="T48" s="56"/>
+    </row>
+    <row r="49" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="55"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="56"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="56"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="56"/>
+      <c r="N49" s="56"/>
+      <c r="O49" s="56"/>
+      <c r="P49" s="56"/>
+      <c r="Q49" s="56"/>
+      <c r="R49" s="56"/>
+      <c r="S49" s="56"/>
+      <c r="T49" s="56"/>
+    </row>
+    <row r="50" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="55"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="56"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="56"/>
+      <c r="L50" s="56"/>
+      <c r="M50" s="56"/>
+      <c r="N50" s="56"/>
+      <c r="O50" s="56"/>
+      <c r="P50" s="56"/>
+      <c r="Q50" s="56"/>
+      <c r="R50" s="56"/>
+      <c r="S50" s="56"/>
+      <c r="T50" s="56"/>
+    </row>
+    <row r="51" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="55"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="56"/>
+      <c r="N51" s="56"/>
+      <c r="O51" s="56"/>
+      <c r="P51" s="56"/>
+      <c r="Q51" s="56"/>
+      <c r="R51" s="56"/>
+      <c r="S51" s="56"/>
+      <c r="T51" s="56"/>
+    </row>
+    <row r="52" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="55"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="56"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="56"/>
+      <c r="L52" s="56"/>
+      <c r="M52" s="56"/>
+      <c r="N52" s="56"/>
+      <c r="O52" s="56"/>
+      <c r="P52" s="56"/>
+      <c r="Q52" s="56"/>
+      <c r="R52" s="56"/>
+      <c r="S52" s="56"/>
+      <c r="T52" s="56"/>
+    </row>
+    <row r="53" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="55"/>
+    </row>
+    <row r="54" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="55"/>
+    </row>
+    <row r="55" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="55"/>
+    </row>
+    <row r="56" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="55"/>
+    </row>
+    <row r="57" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="55"/>
+    </row>
+    <row r="58" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="55"/>
+    </row>
+    <row r="59" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="55"/>
+    </row>
+    <row r="60" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="55"/>
+    </row>
+    <row r="61" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="55"/>
+    </row>
+    <row r="62" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="55"/>
+    </row>
+    <row r="63" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="55"/>
+    </row>
+    <row r="64" spans="1:20" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="55"/>
+    </row>
+    <row r="65" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="55"/>
+    </row>
+    <row r="66" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="55"/>
+    </row>
+    <row r="67" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="55"/>
+    </row>
+    <row r="68" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="55"/>
+    </row>
+    <row r="69" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="42"/>
+    </row>
+    <row r="70" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="42"/>
+    </row>
+    <row r="71" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="42"/>
+    </row>
+    <row r="72" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="42"/>
+    </row>
+    <row r="73" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="42"/>
+    </row>
+    <row r="74" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="42"/>
+    </row>
+    <row r="75" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="42"/>
+    </row>
+    <row r="76" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="42"/>
+    </row>
+    <row r="77" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="42"/>
+    </row>
+    <row r="78" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="42"/>
+    </row>
+    <row r="79" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="42"/>
+    </row>
+    <row r="80" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="42"/>
+    </row>
+    <row r="81" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="42"/>
+    </row>
+    <row r="82" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="42"/>
+    </row>
+    <row r="83" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="42"/>
+    </row>
+    <row r="84" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="42"/>
+    </row>
+    <row r="85" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="42"/>
+    </row>
+    <row r="86" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="42"/>
+    </row>
+    <row r="87" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="42"/>
+    </row>
+    <row r="88" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="42"/>
+    </row>
+    <row r="89" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="42"/>
+    </row>
+    <row r="90" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="42"/>
+    </row>
+    <row r="91" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="42"/>
+    </row>
+    <row r="92" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="42"/>
+    </row>
+    <row r="93" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="42"/>
+    </row>
+    <row r="94" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="42"/>
+    </row>
+    <row r="95" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="42"/>
+    </row>
+    <row r="96" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="42"/>
+    </row>
+    <row r="97" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="42"/>
+    </row>
+    <row r="98" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="42"/>
+    </row>
+    <row r="99" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="42"/>
+    </row>
+    <row r="100" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="42"/>
+    </row>
+    <row r="101" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="42"/>
+    </row>
+    <row r="102" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="42"/>
+    </row>
+    <row r="103" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="42"/>
+    </row>
+    <row r="104" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="42"/>
+    </row>
+    <row r="105" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="42"/>
+    </row>
+    <row r="106" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="42"/>
+    </row>
+    <row r="107" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="42"/>
+    </row>
+    <row r="108" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="42"/>
+    </row>
+    <row r="109" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="42"/>
+    </row>
+    <row r="110" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="42"/>
+    </row>
+    <row r="111" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="42"/>
+    </row>
+    <row r="112" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="42"/>
+    </row>
+    <row r="113" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="42"/>
+    </row>
+    <row r="114" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="42"/>
+    </row>
+    <row r="115" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="42"/>
+    </row>
+    <row r="116" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="42"/>
+    </row>
+    <row r="117" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117" s="42"/>
+    </row>
+    <row r="118" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118" s="42"/>
+    </row>
+    <row r="119" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119" s="42"/>
+    </row>
+    <row r="120" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="42"/>
+    </row>
+    <row r="121" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121" s="42"/>
+    </row>
+    <row r="122" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="42"/>
+    </row>
+    <row r="123" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="42"/>
+    </row>
+    <row r="124" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="42"/>
+    </row>
+    <row r="125" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125" s="42"/>
+    </row>
+    <row r="126" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A126" s="42"/>
+    </row>
+    <row r="127" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127" s="42"/>
+    </row>
+    <row r="128" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A128" s="42"/>
+    </row>
+    <row r="129" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129" s="42"/>
+    </row>
+    <row r="130" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="42"/>
+    </row>
+    <row r="131" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="42"/>
+    </row>
+    <row r="132" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A132" s="42"/>
+    </row>
+    <row r="133" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133" s="42"/>
+    </row>
+    <row r="134" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="42"/>
+    </row>
+    <row r="135" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="42"/>
+    </row>
+    <row r="136" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136" s="42"/>
+    </row>
+    <row r="137" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A137" s="42"/>
+    </row>
+    <row r="138" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A138" s="42"/>
+    </row>
+    <row r="139" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" s="42"/>
+    </row>
+    <row r="140" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A140" s="42"/>
+    </row>
+    <row r="141" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A141" s="42"/>
+    </row>
+    <row r="142" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A142" s="42"/>
+    </row>
+    <row r="143" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A143" s="42"/>
+    </row>
+    <row r="144" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A144" s="42"/>
+    </row>
+    <row r="145" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A145" s="42"/>
+    </row>
+    <row r="146" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A146" s="42"/>
+    </row>
+    <row r="147" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A147" s="42"/>
+    </row>
+    <row r="148" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A148" s="42"/>
+    </row>
+    <row r="149" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A149" s="42"/>
+    </row>
+    <row r="150" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A150" s="42"/>
+    </row>
+    <row r="151" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A151" s="42"/>
+    </row>
+    <row r="152" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A152" s="42"/>
+    </row>
+    <row r="153" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A153" s="42"/>
+    </row>
+    <row r="154" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A154" s="42"/>
+    </row>
+    <row r="155" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A155" s="42"/>
+    </row>
+    <row r="156" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A156" s="42"/>
+    </row>
+    <row r="157" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A157" s="42"/>
+    </row>
+    <row r="158" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A158" s="42"/>
+    </row>
+    <row r="159" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A159" s="42"/>
+    </row>
+    <row r="160" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A160" s="42"/>
+    </row>
+    <row r="161" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A161" s="42"/>
+    </row>
+    <row r="162" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A162" s="42"/>
+    </row>
+    <row r="163" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A163" s="42"/>
+    </row>
+    <row r="164" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A164" s="42"/>
+    </row>
+    <row r="165" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A165" s="42"/>
+    </row>
+    <row r="166" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A166" s="42"/>
+    </row>
+    <row r="167" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A167" s="42"/>
+    </row>
+    <row r="168" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A168" s="42"/>
+    </row>
+    <row r="169" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A169" s="42"/>
+    </row>
+    <row r="170" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A170" s="42"/>
+    </row>
+    <row r="171" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A171" s="42"/>
+    </row>
+    <row r="172" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A172" s="42"/>
+    </row>
+    <row r="173" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A173" s="42"/>
+    </row>
+    <row r="174" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A174" s="42"/>
+    </row>
+    <row r="175" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A175" s="42"/>
+    </row>
+    <row r="176" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A176" s="42"/>
+    </row>
+    <row r="177" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A177" s="42"/>
+    </row>
+    <row r="178" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A178" s="42"/>
+    </row>
+    <row r="179" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A179" s="42"/>
+    </row>
+    <row r="180" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A180" s="42"/>
+    </row>
+    <row r="181" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A181" s="42"/>
+    </row>
+    <row r="182" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A182" s="42"/>
+    </row>
+    <row r="183" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A183" s="42"/>
+    </row>
+    <row r="184" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A184" s="42"/>
+    </row>
+    <row r="185" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A185" s="42"/>
+    </row>
+    <row r="186" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A186" s="42"/>
+    </row>
+    <row r="187" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A187" s="42"/>
+    </row>
+    <row r="188" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A188" s="42"/>
+    </row>
+    <row r="189" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A189" s="42"/>
+    </row>
+    <row r="190" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A190" s="42"/>
+    </row>
+    <row r="191" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A191" s="42"/>
+    </row>
+    <row r="192" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A192" s="42"/>
+    </row>
+    <row r="193" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A193" s="42"/>
+    </row>
+    <row r="194" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A194" s="42"/>
+    </row>
+    <row r="195" spans="1:1" s="41" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A195" s="42"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="8">
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A13:G13"/>
+  <mergeCells count="10">
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A14:G14"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A1:A2"/>
@@ -5044,33 +5914,33 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D29:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="29" spans="4:9">
-      <c r="D29" s="48" t="s">
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -5085,27 +5955,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B40:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="40" spans="2:7">
-      <c r="B40" s="49" t="s">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Formatting and spelling corrections
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="452" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="452" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="1" r:id="rId1"/>
@@ -256,9 +256,6 @@
     <t>RVM2 Sub-Requirements</t>
   </si>
   <si>
-    <t>RCL-RVM2-1</t>
-  </si>
-  <si>
     <t>RCL-RVM3</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>The spacecraft shall carry visual aids to aid in the primary spacecraft identifying it</t>
   </si>
   <si>
-    <t>RCL-RVM3-1</t>
-  </si>
-  <si>
     <t>The spacecraft shall carry components necessary for the primary spacecraft to accomplish its mission goals</t>
   </si>
   <si>
@@ -283,28 +277,9 @@
     <t>The spacecraft shall be capable of conjoining to another spacecraft of equal size and dimensions prior to, during, and after launch.</t>
   </si>
   <si>
-    <r>
-      <t>The mechanism used for separation shall be capable of accieving an intial spacecraft rotational rate no greater than 10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>°/s</t>
-    </r>
-  </si>
-  <si>
-    <t>RCL-RVM3-1-1</t>
-  </si>
-  <si>
     <t>The spacecraft shall be capable of withstanding the loads and conditions associated with its launch environment.</t>
   </si>
   <si>
-    <t>RCL-RVM2-2</t>
-  </si>
-  <si>
     <t>The spacecraft shall allow for the visual aid system to be remotely commanded to be powered on and off.</t>
   </si>
   <si>
@@ -351,13 +326,28 @@
   </si>
   <si>
     <t>RCL-RVM4</t>
+  </si>
+  <si>
+    <t>The mechanism used for separation shall be capable of achieving an initial spacecraft rotational rate no greater than 10°/s</t>
+  </si>
+  <si>
+    <t>RCL2-RVM2-1</t>
+  </si>
+  <si>
+    <t>RCL2-RVM2-2</t>
+  </si>
+  <si>
+    <t>RCL2-RVM3-1</t>
+  </si>
+  <si>
+    <t>RCL2-RVM3-1-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -402,11 +392,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -693,6 +678,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -702,82 +710,59 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -803,7 +788,102 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -827,102 +907,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1113,14 +1098,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E10"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Revision" dataDxfId="6"/>
-    <tableColumn id="2" name="Release Date" dataDxfId="5"/>
-    <tableColumn id="3" name="Brief Revision Comment" dataDxfId="4"/>
-    <tableColumn id="4" name="Author" dataDxfId="3"/>
-    <tableColumn id="5" name="Approval" dataDxfId="2"/>
+    <tableColumn id="1" name="Revision" dataDxfId="4"/>
+    <tableColumn id="2" name="Release Date" dataDxfId="3"/>
+    <tableColumn id="3" name="Brief Revision Comment" dataDxfId="2"/>
+    <tableColumn id="4" name="Author" dataDxfId="1"/>
+    <tableColumn id="5" name="Approval" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1473,85 +1458,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="27">
         <v>41582</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="16" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="16"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="B8" s="25"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1559,7 +1544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -1567,7 +1552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1575,7 +1560,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1583,7 +1568,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1591,7 +1576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -1599,7 +1584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
@@ -1607,7 +1592,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
@@ -1615,7 +1600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -1623,7 +1608,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
@@ -1631,7 +1616,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -1639,7 +1624,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -1647,7 +1632,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30">
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
@@ -1655,7 +1640,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30">
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
@@ -1663,7 +1648,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
@@ -1671,7 +1656,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
@@ -1679,7 +1664,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>42</v>
       </c>
@@ -1687,7 +1672,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
@@ -1695,7 +1680,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
@@ -1703,63 +1688,63 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
     </row>
@@ -1781,14 +1766,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1797,123 +1782,123 @@
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="24">
+        <v>41726</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="45">
-        <v>41726</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="44" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="44"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1925,152 +1910,152 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A1" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="35"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="33"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="35"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="33"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="36"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-    </row>
-    <row r="12" spans="1:7" ht="59.25" customHeight="1">
-      <c r="A12" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-    </row>
-    <row r="13" spans="1:7" ht="59.25" customHeight="1">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-    </row>
-    <row r="14" spans="1:7" ht="59.25" customHeight="1">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+    <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="37"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+    </row>
+    <row r="12" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+    </row>
+    <row r="13" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+    </row>
+    <row r="14" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="39"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2084,14 +2069,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60.28515625" style="7" customWidth="1"/>
     <col min="2" max="5" width="9.140625" style="8"/>
@@ -2100,52 +2085,52 @@
     <col min="8" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="41" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="43"/>
+      <c r="B2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="21"/>
-    </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="F2" s="43"/>
+      <c r="G2" s="41"/>
+    </row>
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:7" ht="30">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>60</v>
       </c>
@@ -2166,7 +2151,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>70</v>
       </c>
@@ -2187,9 +2172,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>53</v>
@@ -2207,12 +2192,12 @@
         <v>36</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -2221,24 +2206,24 @@
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="14.25">
-      <c r="A8" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-    </row>
-    <row r="9" spans="1:7" ht="30">
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>62</v>
       </c>
@@ -2257,9 +2242,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>53</v>
@@ -2278,7 +2263,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>71</v>
       </c>
@@ -2295,18 +2280,18 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25">
-      <c r="A12" s="25" t="s">
+    <row r="12" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-    </row>
-    <row r="13" spans="1:7" s="12" customFormat="1" ht="30">
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+    </row>
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>66</v>
       </c>
@@ -2327,7 +2312,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="30">
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>69</v>
       </c>
@@ -2348,18 +2333,18 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="15">
-      <c r="A15" s="25" t="s">
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-    </row>
-    <row r="16" spans="1:7" s="12" customFormat="1" ht="45">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+    </row>
+    <row r="16" spans="1:7" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>74</v>
       </c>
@@ -2380,9 +2365,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="12" customFormat="1" ht="30">
+    <row r="17" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>53</v>
@@ -2414,16 +2399,16 @@
       <c r="S17" s="15"/>
       <c r="T17" s="15"/>
     </row>
-    <row r="18" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A18" s="24" t="s">
+    <row r="18" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
@@ -2438,9 +2423,9 @@
       <c r="S18" s="15"/>
       <c r="T18" s="15"/>
     </row>
-    <row r="19" spans="1:20" s="12" customFormat="1" ht="30">
+    <row r="19" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
@@ -2454,7 +2439,7 @@
         <v>36</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
@@ -2470,9 +2455,9 @@
       <c r="S19" s="15"/>
       <c r="T19" s="15"/>
     </row>
-    <row r="20" spans="1:20" s="12" customFormat="1" ht="30">
+    <row r="20" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>53</v>
@@ -2488,7 +2473,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
@@ -2504,16 +2489,16 @@
       <c r="S20" s="15"/>
       <c r="T20" s="15"/>
     </row>
-    <row r="21" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A21" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
+    <row r="21" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
@@ -2528,9 +2513,9 @@
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
     </row>
-    <row r="22" spans="1:20" s="12" customFormat="1" ht="30">
+    <row r="22" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -2544,7 +2529,7 @@
         <v>36</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
@@ -2560,16 +2545,16 @@
       <c r="S22" s="15"/>
       <c r="T22" s="15"/>
     </row>
-    <row r="23" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A23" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
+    <row r="23" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
@@ -2584,9 +2569,9 @@
       <c r="S23" s="15"/>
       <c r="T23" s="15"/>
     </row>
-    <row r="24" spans="1:20" s="12" customFormat="1" ht="30">
+    <row r="24" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>53</v>
@@ -2600,7 +2585,7 @@
         <v>36</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
@@ -2616,9 +2601,9 @@
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
     </row>
-    <row r="25" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="25" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2640,7 +2625,7 @@
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
     </row>
-    <row r="26" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="26" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -2662,7 +2647,7 @@
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
     </row>
-    <row r="27" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="27" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -2684,7 +2669,7 @@
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
     </row>
-    <row r="28" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="28" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -2706,7 +2691,7 @@
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
     </row>
-    <row r="29" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="29" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2728,7 +2713,7 @@
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
     </row>
-    <row r="30" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="30" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2750,7 +2735,7 @@
       <c r="S30" s="15"/>
       <c r="T30" s="15"/>
     </row>
-    <row r="31" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="31" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2772,7 +2757,7 @@
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
     </row>
-    <row r="32" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="32" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2794,7 +2779,7 @@
       <c r="S32" s="15"/>
       <c r="T32" s="15"/>
     </row>
-    <row r="33" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="33" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2816,7 +2801,7 @@
       <c r="S33" s="15"/>
       <c r="T33" s="15"/>
     </row>
-    <row r="34" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="34" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -2838,7 +2823,7 @@
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
     </row>
-    <row r="35" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="35" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -2860,7 +2845,7 @@
       <c r="S35" s="15"/>
       <c r="T35" s="15"/>
     </row>
-    <row r="36" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="36" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2882,7 +2867,7 @@
       <c r="S36" s="15"/>
       <c r="T36" s="15"/>
     </row>
-    <row r="37" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="37" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -2904,7 +2889,7 @@
       <c r="S37" s="15"/>
       <c r="T37" s="15"/>
     </row>
-    <row r="38" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="38" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2926,7 +2911,7 @@
       <c r="S38" s="15"/>
       <c r="T38" s="15"/>
     </row>
-    <row r="39" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="39" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -2948,7 +2933,7 @@
       <c r="S39" s="15"/>
       <c r="T39" s="15"/>
     </row>
-    <row r="40" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="40" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -2970,7 +2955,7 @@
       <c r="S40" s="15"/>
       <c r="T40" s="15"/>
     </row>
-    <row r="41" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="41" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -2992,7 +2977,7 @@
       <c r="S41" s="15"/>
       <c r="T41" s="15"/>
     </row>
-    <row r="42" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="42" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -3014,7 +2999,7 @@
       <c r="S42" s="15"/>
       <c r="T42" s="15"/>
     </row>
-    <row r="43" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="43" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -3036,7 +3021,7 @@
       <c r="S43" s="15"/>
       <c r="T43" s="15"/>
     </row>
-    <row r="44" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="44" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -3058,7 +3043,7 @@
       <c r="S44" s="15"/>
       <c r="T44" s="15"/>
     </row>
-    <row r="45" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="45" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -3080,7 +3065,7 @@
       <c r="S45" s="15"/>
       <c r="T45" s="15"/>
     </row>
-    <row r="46" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="46" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -3102,7 +3087,7 @@
       <c r="S46" s="15"/>
       <c r="T46" s="15"/>
     </row>
-    <row r="47" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="47" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -3124,7 +3109,7 @@
       <c r="S47" s="15"/>
       <c r="T47" s="15"/>
     </row>
-    <row r="48" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="48" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -3146,7 +3131,7 @@
       <c r="S48" s="15"/>
       <c r="T48" s="15"/>
     </row>
-    <row r="49" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="49" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -3168,7 +3153,7 @@
       <c r="S49" s="15"/>
       <c r="T49" s="15"/>
     </row>
-    <row r="50" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="50" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -3190,7 +3175,7 @@
       <c r="S50" s="15"/>
       <c r="T50" s="15"/>
     </row>
-    <row r="51" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="51" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
@@ -3212,7 +3197,7 @@
       <c r="S51" s="15"/>
       <c r="T51" s="15"/>
     </row>
-    <row r="52" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="52" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
@@ -3234,7 +3219,7 @@
       <c r="S52" s="15"/>
       <c r="T52" s="15"/>
     </row>
-    <row r="53" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="53" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -3256,7 +3241,7 @@
       <c r="S53" s="15"/>
       <c r="T53" s="15"/>
     </row>
-    <row r="54" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="54" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
@@ -3278,433 +3263,433 @@
       <c r="S54" s="15"/>
       <c r="T54" s="15"/>
     </row>
-    <row r="55" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="55" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
     </row>
-    <row r="56" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="56" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
     </row>
-    <row r="57" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="57" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14"/>
     </row>
-    <row r="58" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="58" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14"/>
     </row>
-    <row r="59" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="59" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
     </row>
-    <row r="60" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="60" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
     </row>
-    <row r="61" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="61" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
     </row>
-    <row r="62" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="62" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
     </row>
-    <row r="63" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="63" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
     </row>
-    <row r="64" spans="1:20" s="12" customFormat="1" ht="15">
+    <row r="64" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
     </row>
-    <row r="65" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="65" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
     </row>
-    <row r="66" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="66" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
     </row>
-    <row r="67" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="67" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
     </row>
-    <row r="68" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="68" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14"/>
     </row>
-    <row r="69" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="69" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14"/>
     </row>
-    <row r="70" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="70" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14"/>
     </row>
-    <row r="71" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="71" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
     </row>
-    <row r="72" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="72" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
     </row>
-    <row r="73" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="73" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
     </row>
-    <row r="74" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="74" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
     </row>
-    <row r="75" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="75" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
     </row>
-    <row r="76" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="76" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="13"/>
     </row>
-    <row r="77" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="77" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="13"/>
     </row>
-    <row r="78" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="78" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
     </row>
-    <row r="79" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="79" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
     </row>
-    <row r="80" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="80" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="13"/>
     </row>
-    <row r="81" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="81" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="13"/>
     </row>
-    <row r="82" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="82" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="13"/>
     </row>
-    <row r="83" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="83" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="13"/>
     </row>
-    <row r="84" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="84" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
     </row>
-    <row r="85" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="85" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="13"/>
     </row>
-    <row r="86" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="86" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="13"/>
     </row>
-    <row r="87" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="87" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="13"/>
     </row>
-    <row r="88" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="88" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
     </row>
-    <row r="89" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="89" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
     </row>
-    <row r="90" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="90" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="13"/>
     </row>
-    <row r="91" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="91" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
     </row>
-    <row r="92" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="92" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
     </row>
-    <row r="93" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="93" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
     </row>
-    <row r="94" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="94" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
     </row>
-    <row r="95" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="95" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="13"/>
     </row>
-    <row r="96" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="96" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="13"/>
     </row>
-    <row r="97" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="97" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
     </row>
-    <row r="98" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="98" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
     </row>
-    <row r="99" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="99" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="13"/>
     </row>
-    <row r="100" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="100" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
     </row>
-    <row r="101" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="101" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
     </row>
-    <row r="102" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="102" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="13"/>
     </row>
-    <row r="103" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="103" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="13"/>
     </row>
-    <row r="104" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="104" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="13"/>
     </row>
-    <row r="105" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="105" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="13"/>
     </row>
-    <row r="106" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="106" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="13"/>
     </row>
-    <row r="107" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="107" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
     </row>
-    <row r="108" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="108" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="13"/>
     </row>
-    <row r="109" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="109" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="13"/>
     </row>
-    <row r="110" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="110" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="13"/>
     </row>
-    <row r="111" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="111" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="13"/>
     </row>
-    <row r="112" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="112" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="13"/>
     </row>
-    <row r="113" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="113" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="13"/>
     </row>
-    <row r="114" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="114" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
     </row>
-    <row r="115" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="115" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="13"/>
     </row>
-    <row r="116" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="116" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
     </row>
-    <row r="117" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="117" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
     </row>
-    <row r="118" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="118" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
     </row>
-    <row r="119" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="119" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="13"/>
     </row>
-    <row r="120" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="120" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="13"/>
     </row>
-    <row r="121" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="121" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="13"/>
     </row>
-    <row r="122" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="122" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="13"/>
     </row>
-    <row r="123" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="123" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
     </row>
-    <row r="124" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="124" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="13"/>
     </row>
-    <row r="125" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="125" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
     </row>
-    <row r="126" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="126" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
     </row>
-    <row r="127" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="127" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="13"/>
     </row>
-    <row r="128" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="128" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
     </row>
-    <row r="129" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="129" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="13"/>
     </row>
-    <row r="130" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="130" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="13"/>
     </row>
-    <row r="131" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="131" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="13"/>
     </row>
-    <row r="132" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="132" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="13"/>
     </row>
-    <row r="133" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="133" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="13"/>
     </row>
-    <row r="134" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="134" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
     </row>
-    <row r="135" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="135" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="13"/>
     </row>
-    <row r="136" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="136" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="13"/>
     </row>
-    <row r="137" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="137" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="13"/>
     </row>
-    <row r="138" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="138" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="13"/>
     </row>
-    <row r="139" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="139" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="13"/>
     </row>
-    <row r="140" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="140" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="13"/>
     </row>
-    <row r="141" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="141" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="13"/>
     </row>
-    <row r="142" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="142" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="13"/>
     </row>
-    <row r="143" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="143" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="13"/>
     </row>
-    <row r="144" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="144" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
     </row>
-    <row r="145" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="145" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="13"/>
     </row>
-    <row r="146" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="146" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="13"/>
     </row>
-    <row r="147" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="147" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="13"/>
     </row>
-    <row r="148" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="148" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="13"/>
     </row>
-    <row r="149" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="149" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
     </row>
-    <row r="150" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="150" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="13"/>
     </row>
-    <row r="151" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="151" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="13"/>
     </row>
-    <row r="152" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="152" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="13"/>
     </row>
-    <row r="153" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="153" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="13"/>
     </row>
-    <row r="154" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="154" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="13"/>
     </row>
-    <row r="155" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="155" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="13"/>
     </row>
-    <row r="156" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="156" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="13"/>
     </row>
-    <row r="157" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="157" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
     </row>
-    <row r="158" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="158" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="13"/>
     </row>
-    <row r="159" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="159" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="13"/>
     </row>
-    <row r="160" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="160" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="13"/>
     </row>
-    <row r="161" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="161" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="13"/>
     </row>
-    <row r="162" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="162" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="13"/>
     </row>
-    <row r="163" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="163" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
     </row>
-    <row r="164" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="164" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="13"/>
     </row>
-    <row r="165" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="165" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="13"/>
     </row>
-    <row r="166" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="166" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="13"/>
     </row>
-    <row r="167" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="167" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="13"/>
     </row>
-    <row r="168" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="168" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="13"/>
     </row>
-    <row r="169" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="169" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="13"/>
     </row>
-    <row r="170" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="170" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
     </row>
-    <row r="171" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="171" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="13"/>
     </row>
-    <row r="172" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="172" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="13"/>
     </row>
-    <row r="173" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="173" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
     </row>
-    <row r="174" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="174" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="13"/>
     </row>
-    <row r="175" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="175" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="13"/>
     </row>
-    <row r="176" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="176" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="13"/>
     </row>
-    <row r="177" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="177" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="13"/>
     </row>
-    <row r="178" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="178" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="13"/>
     </row>
-    <row r="179" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="179" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
     </row>
-    <row r="180" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="180" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="13"/>
     </row>
-    <row r="181" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="181" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="13"/>
     </row>
-    <row r="182" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="182" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
     </row>
-    <row r="183" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="183" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="13"/>
     </row>
-    <row r="184" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="184" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
     </row>
-    <row r="185" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="185" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="13"/>
     </row>
-    <row r="186" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="186" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="13"/>
     </row>
-    <row r="187" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="187" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="13"/>
     </row>
-    <row r="188" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="188" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="13"/>
     </row>
-    <row r="189" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="189" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="13"/>
     </row>
-    <row r="190" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="190" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="13"/>
     </row>
-    <row r="191" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="191" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
     </row>
-    <row r="192" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="192" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="13"/>
     </row>
-    <row r="193" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="193" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="13"/>
     </row>
-    <row r="194" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="194" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="13"/>
     </row>
-    <row r="195" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="195" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="13"/>
     </row>
-    <row r="196" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="196" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="13"/>
     </row>
-    <row r="197" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="197" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a bunch of changes that swartwout recommended
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="452" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="452" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="116">
   <si>
     <t>Document Title</t>
   </si>
@@ -196,63 +196,12 @@
     <t xml:space="preserve">Task Number </t>
   </si>
   <si>
-    <t>RCL2-RVM1</t>
-  </si>
-  <si>
-    <t>RCL2-RVM2</t>
-  </si>
-  <si>
-    <t>The spacecraft shall be capable of integrating into a 6U CubeSat deployer</t>
-  </si>
-  <si>
     <t>RVM1 Sub-Requirements</t>
   </si>
   <si>
-    <t>Spacecraft size and dimensions shall conform to the CubeSat Design Specification for a 3U Spacecraft</t>
-  </si>
-  <si>
-    <t>RCL2-RVM1-1</t>
-  </si>
-  <si>
-    <t>RCL2-RVM1-2</t>
-  </si>
-  <si>
     <t>RVM1-2 Sub-Requirements</t>
   </si>
   <si>
-    <t>The mechanism used for conjoining each spacecraft shall be capable of withstanding all launch vehicle ejection loads.</t>
-  </si>
-  <si>
-    <t>RCL2-RVM1-2-1</t>
-  </si>
-  <si>
-    <t>RCL2-RVM1-2-2</t>
-  </si>
-  <si>
-    <t>The secondary spacecraft shall remain in a powered off state until separation.</t>
-  </si>
-  <si>
-    <t>The spacecraft shall be capable of supporting a mission lifetime of at least two weeks</t>
-  </si>
-  <si>
-    <t>There shall be a mechanism in place that allows for the separation of each spacecraft.</t>
-  </si>
-  <si>
-    <t>RCL2-RVM1-3</t>
-  </si>
-  <si>
-    <t>RVM1-3 Sub-Requirements</t>
-  </si>
-  <si>
-    <t>The mechanism used for separation shall be capable of achieving an initial relative separation velocity between each spacecraft no greater than 1 m/s</t>
-  </si>
-  <si>
-    <t>RCL2-RVM1-3-1</t>
-  </si>
-  <si>
-    <t>RCL2-RVM1-3-2</t>
-  </si>
-  <si>
     <t>RVM2 Sub-Requirements</t>
   </si>
   <si>
@@ -262,30 +211,6 @@
     <t>RVM3 Sub-Requirements</t>
   </si>
   <si>
-    <t>The spacecraft shall carry visual aids to aid in the primary spacecraft identifying it</t>
-  </si>
-  <si>
-    <t>The spacecraft shall carry components necessary for the primary spacecraft to accomplish its mission goals</t>
-  </si>
-  <si>
-    <t>RVM3-1 Sub-Requirements</t>
-  </si>
-  <si>
-    <t>The spacecraft shall have a power system capable of powering the spacecraft for the entirety of its two week mission life.</t>
-  </si>
-  <si>
-    <t>The spacecraft shall be capable of conjoining to another spacecraft of equal size and dimensions prior to, during, and after launch.</t>
-  </si>
-  <si>
-    <t>The spacecraft shall be capable of withstanding the loads and conditions associated with its launch environment.</t>
-  </si>
-  <si>
-    <t>The spacecraft shall allow for the visual aid system to be remotely commanded to be powered on and off.</t>
-  </si>
-  <si>
-    <t>\</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -319,35 +244,192 @@
     <t xml:space="preserve">This document is organized in such a manner that Top-Level requirements (such as mission sizing and lifetime constraints) are listed at the top of the matrix, with all other requirements (such as power and separation constraints) being derived from these top level requirements.                                                         The distinction between each level of requirements is indicated by the task number associated with each requirement. A top level requirement, for example, would have a task number of RCL2-RVM1, while a sub-requirement of said requirement would have a number of RCL2-RVM1-1, and so on.                              Each requirement also has one or more verification methods associated with verifying that it is met. These methods consist of Analysis (CAD Analysis, mathematical calculations, etc), Test (Vibration, Functional, Thermal Testing), Demo (Antenna Deployment, Propulsive Measurements, etc.), and Exmine (Measurements, visual inspecton, etc). </t>
   </si>
   <si>
-    <t>A Secondary Spacecraft missions operation document shall be supplied to Boeing that documents the operation of the secondary spacecraft</t>
-  </si>
-  <si>
     <t>AS&amp;IS</t>
   </si>
   <si>
     <t>RCL-RVM4</t>
   </si>
   <si>
-    <t>The mechanism used for separation shall be capable of achieving an initial spacecraft rotational rate no greater than 10°/s</t>
-  </si>
-  <si>
-    <t>RCL2-RVM2-1</t>
-  </si>
-  <si>
-    <t>RCL2-RVM2-2</t>
-  </si>
-  <si>
-    <t>RCL2-RVM3-1</t>
-  </si>
-  <si>
-    <t>RCL2-RVM3-1-1</t>
+    <t>RCL-RVM1</t>
+  </si>
+  <si>
+    <t>RCL-RVM2</t>
+  </si>
+  <si>
+    <t>The Rascal mission shall consist of a primary spacecraft (Jade) that will perform rendezvous and proximity operations realtive to a target resident space object (Nephrite).</t>
+  </si>
+  <si>
+    <t>The RSO and primary spacecraft shall separate with a relative speed no more than 1 m/s, with a  goal of 5 cm/s.</t>
+  </si>
+  <si>
+    <t>RCL-RVM3-1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The RSO  shall separate from the primary spacecraft with a rotational rate no more than 10 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>⁰</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/s, with a  goal of 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>⁰</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>/s.</t>
+    </r>
+  </si>
+  <si>
+    <t>RCL-RVM1-1</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-2</t>
+  </si>
+  <si>
+    <t>The RSO shall physically separate from the primary spacecraft upon command from the ground.</t>
+  </si>
+  <si>
+    <t>Both the RSO and primary spacecraft shall be physically conjoined prior to launch.</t>
+  </si>
+  <si>
+    <t>Both the RSO and primary spacecraft shall be physically conjoined during launch.</t>
+  </si>
+  <si>
+    <t>RCL-RVM5</t>
+  </si>
+  <si>
+    <t>Both the RSO and primary spacecraft shall be physically conjoined during launch vehicle separation.</t>
+  </si>
+  <si>
+    <t>RCL-RVM6</t>
+  </si>
+  <si>
+    <t>Both the RSO and primary spacecraft shall integrate into the same 6U CubeSat Deployer.</t>
+  </si>
+  <si>
+    <t>RCL-RVM2-1</t>
+  </si>
+  <si>
+    <t>RVM5 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>RCL-RVM5-1</t>
+  </si>
+  <si>
+    <t>RVM5-1 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>RCL-RVM5-1-1</t>
+  </si>
+  <si>
+    <t>RCL-RVM5-1-2</t>
+  </si>
+  <si>
+    <t>RVM4 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>RCL-RVM4-1</t>
+  </si>
+  <si>
+    <t>Both the RSO and primary spacecraft shall be physically conjoined during initial on-orbit operations.</t>
+  </si>
+  <si>
+    <t>The method used to conjoin the RSO and primary spacecraft shall withstand the loads associated with the launch vehicle environment, as specified by the LSP or by the Proto-Qualification NASA GEVS Random Vibration Profile.</t>
+  </si>
+  <si>
+    <t>The method used to conjoin the RSO and primary spacecraft shall withstand the impulsive load associated with a 2 m/s launch ejection speed.</t>
+  </si>
+  <si>
+    <t>The primary spacecraft shall utilize a propulsion system to execute all RPO maneuvers.</t>
+  </si>
+  <si>
+    <t>The primary spacecraft shall resolve the relative distance and angle between the RSO and primary spacecraft over a range of 0.1-100 meters, with a maximum goal of 2000 meters.</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-1-1</t>
+  </si>
+  <si>
+    <t>RVM1-1 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>The RSO's navigation aids shall be able to be remotely powered on and off.</t>
+  </si>
+  <si>
+    <t>The RSO shall provide navigation aids to the primary spacecraft, as specified in the RCL-O-ADC1 ADC Overview document.</t>
+  </si>
+  <si>
+    <t>The RSO shall operate for a period of two weeks after separation, with a goal of four weeks.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The propulsion system shall provide a total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>V capability of 50 m/s, with a  goal of 100 m/s</t>
+    </r>
+  </si>
+  <si>
+    <t>The propulsion system shall provide 3 Degree of Freedom motion.</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-1-2</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-2-1</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-2-2</t>
+  </si>
+  <si>
+    <t>The system used for primary spacecraft navigation shall be able to integrate into the Colony-II bus.</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-1-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -418,6 +500,17 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.35"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -643,7 +736,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -764,6 +857,12 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -788,7 +887,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -807,7 +906,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -826,7 +925,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -845,7 +944,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -864,7 +963,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -883,7 +982,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -907,7 +1006,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1458,19 +1557,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1482,7 +1581,7 @@
       <c r="E1" s="26"/>
       <c r="F1" s="26"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1494,7 +1593,7 @@
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1506,7 +1605,7 @@
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1518,7 +1617,7 @@
       <c r="E4" s="26"/>
       <c r="F4" s="26"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1530,13 +1629,13 @@
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="25"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1544,7 +1643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -1552,7 +1651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1560,7 +1659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1568,7 +1667,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1576,7 +1675,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -1584,7 +1683,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
@@ -1592,7 +1691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
@@ -1600,7 +1699,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -1608,7 +1707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
@@ -1616,7 +1715,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -1624,7 +1723,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -1632,7 +1731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="30">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
@@ -1640,7 +1739,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="30">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
@@ -1648,7 +1747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
@@ -1656,7 +1755,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
@@ -1664,7 +1763,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="4" t="s">
         <v>42</v>
       </c>
@@ -1672,7 +1771,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
@@ -1680,7 +1779,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
@@ -1688,63 +1787,63 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
     </row>
@@ -1766,14 +1865,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1782,24 +1881,24 @@
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="23" t="s">
         <v>7</v>
       </c>
@@ -1807,93 +1906,93 @@
         <v>41726</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -1910,22 +2009,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="25.5" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1934,9 +2033,9 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="29" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -1945,7 +2044,7 @@
       <c r="F2" s="30"/>
       <c r="G2" s="31"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="32"/>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
@@ -1954,7 +2053,7 @@
       <c r="F3" s="33"/>
       <c r="G3" s="34"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="32"/>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
@@ -1963,7 +2062,7 @@
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="32"/>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
@@ -1972,7 +2071,7 @@
       <c r="F5" s="33"/>
       <c r="G5" s="34"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="32"/>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -1981,7 +2080,7 @@
       <c r="F6" s="33"/>
       <c r="G6" s="34"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="32"/>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
@@ -1990,7 +2089,7 @@
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="32"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -1999,7 +2098,7 @@
       <c r="F8" s="33"/>
       <c r="G8" s="34"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="35"/>
       <c r="B9" s="36"/>
       <c r="C9" s="36"/>
@@ -2008,7 +2107,7 @@
       <c r="F9" s="36"/>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -2017,9 +2116,9 @@
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="38" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -2028,9 +2127,9 @@
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
     </row>
-    <row r="12" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="59.25" customHeight="1">
       <c r="A12" s="39" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
@@ -2039,7 +2138,7 @@
       <c r="F12" s="39"/>
       <c r="G12" s="39"/>
     </row>
-    <row r="13" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="59.25" customHeight="1">
       <c r="A13" s="39"/>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
@@ -2048,7 +2147,7 @@
       <c r="F13" s="39"/>
       <c r="G13" s="39"/>
     </row>
-    <row r="14" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="59.25" customHeight="1">
       <c r="A14" s="39"/>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -2069,14 +2168,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T197"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T203"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="60.28515625" style="7" customWidth="1"/>
     <col min="2" max="5" width="9.140625" style="8"/>
@@ -2085,7 +2185,7 @@
     <col min="8" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="14.25">
       <c r="A1" s="43" t="s">
         <v>48</v>
       </c>
@@ -2102,7 +2202,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="14.25">
       <c r="A2" s="43"/>
       <c r="B2" s="16" t="s">
         <v>49</v>
@@ -2119,7 +2219,7 @@
       <c r="F2" s="43"/>
       <c r="G2" s="41"/>
     </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3" s="42" t="s">
         <v>56</v>
       </c>
@@ -2130,30 +2230,26 @@
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>20</v>
+    <row r="4" spans="1:7" ht="45">
+      <c r="A4" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>36</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="9" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>53</v>
@@ -2164,17 +2260,19 @@
       <c r="D5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="F5" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="9" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>53</v>
@@ -2192,161 +2290,175 @@
         <v>36</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30">
+      <c r="A8" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="B8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30">
+      <c r="A9" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="D9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.25">
+      <c r="A10" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+    </row>
+    <row r="11" spans="1:7" ht="45">
+      <c r="A11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30">
+      <c r="A12" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-    </row>
-    <row r="13" spans="1:7" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="G12" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.25">
+      <c r="A13" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+    </row>
+    <row r="14" spans="1:7" ht="30">
+      <c r="A14" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30">
+      <c r="A15" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-    </row>
-    <row r="16" spans="1:7" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>74</v>
+      <c r="G15" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30">
+      <c r="A16" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>53</v>
@@ -2362,119 +2474,68 @@
         <v>36</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-    </row>
-    <row r="18" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-    </row>
-    <row r="19" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" s="10"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="14.25">
+      <c r="A17" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+    </row>
+    <row r="18" spans="1:20" ht="27">
+      <c r="A18" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="15">
+      <c r="A19" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="C19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="D19" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
-    </row>
-    <row r="20" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>104</v>
-      </c>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" s="12" customFormat="1" ht="15">
+      <c r="A20" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
@@ -2489,16 +2550,24 @@
       <c r="S20" s="15"/>
       <c r="T20" s="15"/>
     </row>
-    <row r="21" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
+    <row r="21" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A21" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
@@ -2513,24 +2582,16 @@
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
     </row>
-    <row r="22" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>105</v>
-      </c>
+    <row r="22" spans="1:20" s="12" customFormat="1" ht="15">
+      <c r="A22" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
@@ -2545,16 +2606,22 @@
       <c r="S22" s="15"/>
       <c r="T22" s="15"/>
     </row>
-    <row r="23" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
+    <row r="23" spans="1:20" s="12" customFormat="1" ht="60">
+      <c r="A23" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
@@ -2569,24 +2636,16 @@
       <c r="S23" s="15"/>
       <c r="T23" s="15"/>
     </row>
-    <row r="24" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>106</v>
-      </c>
+    <row r="24" spans="1:20" s="12" customFormat="1" ht="15">
+      <c r="A24" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
@@ -2601,16 +2660,24 @@
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
     </row>
-    <row r="25" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
+    <row r="25" spans="1:20" s="12" customFormat="1" ht="45">
+      <c r="A25" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
@@ -2625,14 +2692,16 @@
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
     </row>
-    <row r="26" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+    <row r="26" spans="1:20" s="12" customFormat="1" ht="15">
+      <c r="A26" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
@@ -2647,14 +2716,24 @@
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
     </row>
-    <row r="27" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+    <row r="27" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A27" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
@@ -2669,14 +2748,16 @@
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
     </row>
-    <row r="28" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
+    <row r="28" spans="1:20" s="12" customFormat="1" ht="15">
+      <c r="A28" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
@@ -2691,14 +2772,24 @@
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
     </row>
-    <row r="29" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
+    <row r="29" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A29" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>95</v>
+      </c>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
@@ -2713,14 +2804,24 @@
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
     </row>
-    <row r="30" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
+    <row r="30" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A30" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
@@ -2735,7 +2836,7 @@
       <c r="S30" s="15"/>
       <c r="T30" s="15"/>
     </row>
-    <row r="31" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2757,7 +2858,7 @@
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
     </row>
-    <row r="32" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2779,7 +2880,7 @@
       <c r="S32" s="15"/>
       <c r="T32" s="15"/>
     </row>
-    <row r="33" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2801,7 +2902,7 @@
       <c r="S33" s="15"/>
       <c r="T33" s="15"/>
     </row>
-    <row r="34" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A34" s="14"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -2823,7 +2924,7 @@
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
     </row>
-    <row r="35" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -2845,7 +2946,7 @@
       <c r="S35" s="15"/>
       <c r="T35" s="15"/>
     </row>
-    <row r="36" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A36" s="14"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2867,7 +2968,7 @@
       <c r="S36" s="15"/>
       <c r="T36" s="15"/>
     </row>
-    <row r="37" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A37" s="14"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -2889,7 +2990,7 @@
       <c r="S37" s="15"/>
       <c r="T37" s="15"/>
     </row>
-    <row r="38" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A38" s="14"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2911,7 +3012,7 @@
       <c r="S38" s="15"/>
       <c r="T38" s="15"/>
     </row>
-    <row r="39" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A39" s="14"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -2933,7 +3034,7 @@
       <c r="S39" s="15"/>
       <c r="T39" s="15"/>
     </row>
-    <row r="40" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A40" s="14"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -2955,7 +3056,7 @@
       <c r="S40" s="15"/>
       <c r="T40" s="15"/>
     </row>
-    <row r="41" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A41" s="14"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -2977,7 +3078,7 @@
       <c r="S41" s="15"/>
       <c r="T41" s="15"/>
     </row>
-    <row r="42" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A42" s="14"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -2999,7 +3100,7 @@
       <c r="S42" s="15"/>
       <c r="T42" s="15"/>
     </row>
-    <row r="43" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A43" s="14"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -3021,7 +3122,7 @@
       <c r="S43" s="15"/>
       <c r="T43" s="15"/>
     </row>
-    <row r="44" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A44" s="14"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -3043,7 +3144,7 @@
       <c r="S44" s="15"/>
       <c r="T44" s="15"/>
     </row>
-    <row r="45" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A45" s="14"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -3065,7 +3166,7 @@
       <c r="S45" s="15"/>
       <c r="T45" s="15"/>
     </row>
-    <row r="46" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A46" s="14"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -3087,7 +3188,7 @@
       <c r="S46" s="15"/>
       <c r="T46" s="15"/>
     </row>
-    <row r="47" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -3109,7 +3210,7 @@
       <c r="S47" s="15"/>
       <c r="T47" s="15"/>
     </row>
-    <row r="48" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -3131,7 +3232,7 @@
       <c r="S48" s="15"/>
       <c r="T48" s="15"/>
     </row>
-    <row r="49" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A49" s="14"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -3153,7 +3254,7 @@
       <c r="S49" s="15"/>
       <c r="T49" s="15"/>
     </row>
-    <row r="50" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A50" s="14"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -3175,7 +3276,7 @@
       <c r="S50" s="15"/>
       <c r="T50" s="15"/>
     </row>
-    <row r="51" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A51" s="14"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
@@ -3197,7 +3298,7 @@
       <c r="S51" s="15"/>
       <c r="T51" s="15"/>
     </row>
-    <row r="52" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A52" s="14"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
@@ -3219,7 +3320,7 @@
       <c r="S52" s="15"/>
       <c r="T52" s="15"/>
     </row>
-    <row r="53" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A53" s="14"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -3241,7 +3342,7 @@
       <c r="S53" s="15"/>
       <c r="T53" s="15"/>
     </row>
-    <row r="54" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A54" s="14"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
@@ -3263,449 +3364,583 @@
       <c r="S54" s="15"/>
       <c r="T54" s="15"/>
     </row>
-    <row r="55" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A55" s="14"/>
-    </row>
-    <row r="56" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
+      <c r="S55" s="15"/>
+      <c r="T55" s="15"/>
+    </row>
+    <row r="56" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A56" s="14"/>
-    </row>
-    <row r="57" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="15"/>
+      <c r="O56" s="15"/>
+      <c r="P56" s="15"/>
+      <c r="Q56" s="15"/>
+      <c r="R56" s="15"/>
+      <c r="S56" s="15"/>
+      <c r="T56" s="15"/>
+    </row>
+    <row r="57" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A57" s="14"/>
-    </row>
-    <row r="58" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="15"/>
+      <c r="R57" s="15"/>
+      <c r="S57" s="15"/>
+      <c r="T57" s="15"/>
+    </row>
+    <row r="58" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A58" s="14"/>
-    </row>
-    <row r="59" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
+      <c r="O58" s="15"/>
+      <c r="P58" s="15"/>
+      <c r="Q58" s="15"/>
+      <c r="R58" s="15"/>
+      <c r="S58" s="15"/>
+      <c r="T58" s="15"/>
+    </row>
+    <row r="59" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A59" s="14"/>
-    </row>
-    <row r="60" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
+      <c r="O59" s="15"/>
+      <c r="P59" s="15"/>
+      <c r="Q59" s="15"/>
+      <c r="R59" s="15"/>
+      <c r="S59" s="15"/>
+      <c r="T59" s="15"/>
+    </row>
+    <row r="60" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A60" s="14"/>
-    </row>
-    <row r="61" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="15"/>
+      <c r="Q60" s="15"/>
+      <c r="R60" s="15"/>
+      <c r="S60" s="15"/>
+      <c r="T60" s="15"/>
+    </row>
+    <row r="61" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A61" s="14"/>
     </row>
-    <row r="62" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A62" s="14"/>
     </row>
-    <row r="63" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A63" s="14"/>
     </row>
-    <row r="64" spans="1:20" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A64" s="14"/>
     </row>
-    <row r="65" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A65" s="14"/>
     </row>
-    <row r="66" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A66" s="14"/>
     </row>
-    <row r="67" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A67" s="14"/>
     </row>
-    <row r="68" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A68" s="14"/>
     </row>
-    <row r="69" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A69" s="14"/>
     </row>
-    <row r="70" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A70" s="14"/>
     </row>
-    <row r="71" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-    </row>
-    <row r="72" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
-    </row>
-    <row r="73" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-    </row>
-    <row r="74" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
-    </row>
-    <row r="75" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
-    </row>
-    <row r="76" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
-    </row>
-    <row r="77" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A71" s="14"/>
+    </row>
+    <row r="72" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A72" s="14"/>
+    </row>
+    <row r="73" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A73" s="14"/>
+    </row>
+    <row r="74" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A74" s="14"/>
+    </row>
+    <row r="75" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A75" s="14"/>
+    </row>
+    <row r="76" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A76" s="14"/>
+    </row>
+    <row r="77" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A77" s="13"/>
     </row>
-    <row r="78" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A78" s="13"/>
     </row>
-    <row r="79" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A79" s="13"/>
     </row>
-    <row r="80" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A80" s="13"/>
     </row>
-    <row r="81" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A81" s="13"/>
     </row>
-    <row r="82" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A82" s="13"/>
     </row>
-    <row r="83" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A83" s="13"/>
     </row>
-    <row r="84" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A84" s="13"/>
     </row>
-    <row r="85" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A85" s="13"/>
     </row>
-    <row r="86" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A86" s="13"/>
     </row>
-    <row r="87" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A87" s="13"/>
     </row>
-    <row r="88" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A88" s="13"/>
     </row>
-    <row r="89" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A89" s="13"/>
     </row>
-    <row r="90" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A90" s="13"/>
     </row>
-    <row r="91" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A91" s="13"/>
     </row>
-    <row r="92" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A92" s="13"/>
     </row>
-    <row r="93" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A93" s="13"/>
     </row>
-    <row r="94" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A94" s="13"/>
     </row>
-    <row r="95" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A95" s="13"/>
     </row>
-    <row r="96" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A96" s="13"/>
     </row>
-    <row r="97" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A97" s="13"/>
     </row>
-    <row r="98" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A98" s="13"/>
     </row>
-    <row r="99" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A99" s="13"/>
     </row>
-    <row r="100" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A100" s="13"/>
     </row>
-    <row r="101" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A101" s="13"/>
     </row>
-    <row r="102" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A102" s="13"/>
     </row>
-    <row r="103" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A103" s="13"/>
     </row>
-    <row r="104" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A104" s="13"/>
     </row>
-    <row r="105" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A105" s="13"/>
     </row>
-    <row r="106" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A106" s="13"/>
     </row>
-    <row r="107" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A107" s="13"/>
     </row>
-    <row r="108" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A108" s="13"/>
     </row>
-    <row r="109" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A109" s="13"/>
     </row>
-    <row r="110" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A110" s="13"/>
     </row>
-    <row r="111" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A111" s="13"/>
     </row>
-    <row r="112" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A112" s="13"/>
     </row>
-    <row r="113" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A113" s="13"/>
     </row>
-    <row r="114" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A114" s="13"/>
     </row>
-    <row r="115" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A115" s="13"/>
     </row>
-    <row r="116" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A116" s="13"/>
     </row>
-    <row r="117" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A117" s="13"/>
     </row>
-    <row r="118" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A118" s="13"/>
     </row>
-    <row r="119" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A119" s="13"/>
     </row>
-    <row r="120" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A120" s="13"/>
     </row>
-    <row r="121" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A121" s="13"/>
     </row>
-    <row r="122" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A122" s="13"/>
     </row>
-    <row r="123" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A123" s="13"/>
     </row>
-    <row r="124" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A124" s="13"/>
     </row>
-    <row r="125" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A125" s="13"/>
     </row>
-    <row r="126" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A126" s="13"/>
     </row>
-    <row r="127" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A127" s="13"/>
     </row>
-    <row r="128" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A128" s="13"/>
     </row>
-    <row r="129" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A129" s="13"/>
     </row>
-    <row r="130" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A130" s="13"/>
     </row>
-    <row r="131" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A131" s="13"/>
     </row>
-    <row r="132" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A132" s="13"/>
     </row>
-    <row r="133" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A133" s="13"/>
     </row>
-    <row r="134" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A134" s="13"/>
     </row>
-    <row r="135" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A135" s="13"/>
     </row>
-    <row r="136" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A136" s="13"/>
     </row>
-    <row r="137" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A137" s="13"/>
     </row>
-    <row r="138" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A138" s="13"/>
     </row>
-    <row r="139" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A139" s="13"/>
     </row>
-    <row r="140" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A140" s="13"/>
     </row>
-    <row r="141" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A141" s="13"/>
     </row>
-    <row r="142" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A142" s="13"/>
     </row>
-    <row r="143" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A143" s="13"/>
     </row>
-    <row r="144" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A144" s="13"/>
     </row>
-    <row r="145" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A145" s="13"/>
     </row>
-    <row r="146" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A146" s="13"/>
     </row>
-    <row r="147" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A147" s="13"/>
     </row>
-    <row r="148" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A148" s="13"/>
     </row>
-    <row r="149" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A149" s="13"/>
     </row>
-    <row r="150" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A150" s="13"/>
     </row>
-    <row r="151" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A151" s="13"/>
     </row>
-    <row r="152" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A152" s="13"/>
     </row>
-    <row r="153" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A153" s="13"/>
     </row>
-    <row r="154" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A154" s="13"/>
     </row>
-    <row r="155" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A155" s="13"/>
     </row>
-    <row r="156" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A156" s="13"/>
     </row>
-    <row r="157" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A157" s="13"/>
     </row>
-    <row r="158" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A158" s="13"/>
     </row>
-    <row r="159" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A159" s="13"/>
     </row>
-    <row r="160" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A160" s="13"/>
     </row>
-    <row r="161" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A161" s="13"/>
     </row>
-    <row r="162" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A162" s="13"/>
     </row>
-    <row r="163" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A163" s="13"/>
     </row>
-    <row r="164" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A164" s="13"/>
     </row>
-    <row r="165" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A165" s="13"/>
     </row>
-    <row r="166" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A166" s="13"/>
     </row>
-    <row r="167" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A167" s="13"/>
     </row>
-    <row r="168" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A168" s="13"/>
     </row>
-    <row r="169" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A169" s="13"/>
     </row>
-    <row r="170" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A170" s="13"/>
     </row>
-    <row r="171" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A171" s="13"/>
     </row>
-    <row r="172" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A172" s="13"/>
     </row>
-    <row r="173" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A173" s="13"/>
     </row>
-    <row r="174" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A174" s="13"/>
     </row>
-    <row r="175" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A175" s="13"/>
     </row>
-    <row r="176" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A176" s="13"/>
     </row>
-    <row r="177" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A177" s="13"/>
     </row>
-    <row r="178" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A178" s="13"/>
     </row>
-    <row r="179" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A179" s="13"/>
     </row>
-    <row r="180" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A180" s="13"/>
     </row>
-    <row r="181" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A181" s="13"/>
     </row>
-    <row r="182" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A182" s="13"/>
     </row>
-    <row r="183" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A183" s="13"/>
     </row>
-    <row r="184" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A184" s="13"/>
     </row>
-    <row r="185" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A185" s="13"/>
     </row>
-    <row r="186" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A186" s="13"/>
     </row>
-    <row r="187" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A187" s="13"/>
     </row>
-    <row r="188" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A188" s="13"/>
     </row>
-    <row r="189" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A189" s="13"/>
     </row>
-    <row r="190" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A190" s="13"/>
     </row>
-    <row r="191" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A191" s="13"/>
     </row>
-    <row r="192" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A192" s="13"/>
     </row>
-    <row r="193" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A193" s="13"/>
     </row>
-    <row r="194" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A194" s="13"/>
     </row>
-    <row r="195" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A195" s="13"/>
     </row>
-    <row r="196" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A196" s="13"/>
     </row>
-    <row r="197" spans="1:1" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A197" s="13"/>
+    </row>
+    <row r="198" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A198" s="13"/>
+    </row>
+    <row r="199" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A199" s="13"/>
+    </row>
+    <row r="200" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A200" s="13"/>
+    </row>
+    <row r="201" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A201" s="13"/>
+    </row>
+    <row r="202" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A202" s="13"/>
+    </row>
+    <row r="203" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A203" s="13"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="11">
-    <mergeCell ref="A23:G23"/>
+  <mergeCells count="13">
+    <mergeCell ref="A17:G17"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed all mentions of RSO to secondary
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="117">
   <si>
     <t>Document Title</t>
   </si>
@@ -256,17 +256,141 @@
     <t>RCL-RVM2</t>
   </si>
   <si>
-    <t>The Rascal mission shall consist of a primary spacecraft (Jade) that will perform rendezvous and proximity operations realtive to a target resident space object (Nephrite).</t>
-  </si>
-  <si>
-    <t>The RSO and primary spacecraft shall separate with a relative speed no more than 1 m/s, with a  goal of 5 cm/s.</t>
-  </si>
-  <si>
     <t>RCL-RVM3-1</t>
   </si>
   <si>
+    <t>RCL-RVM1-1</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-2</t>
+  </si>
+  <si>
+    <t>RCL-RVM5</t>
+  </si>
+  <si>
+    <t>RCL-RVM6</t>
+  </si>
+  <si>
+    <t>RCL-RVM2-1</t>
+  </si>
+  <si>
+    <t>RVM5 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>RCL-RVM5-1</t>
+  </si>
+  <si>
+    <t>RVM5-1 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>RCL-RVM5-1-1</t>
+  </si>
+  <si>
+    <t>RCL-RVM5-1-2</t>
+  </si>
+  <si>
+    <t>RVM4 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>RCL-RVM4-1</t>
+  </si>
+  <si>
+    <t>The primary spacecraft shall utilize a propulsion system to execute all RPO maneuvers.</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-1-1</t>
+  </si>
+  <si>
+    <t>RVM1-1 Sub-Requirements</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">The RSO  shall separate from the primary spacecraft with a rotational rate no more than 10 </t>
+      <t xml:space="preserve">The propulsion system shall provide a total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>V capability of 50 m/s, with a  goal of 100 m/s</t>
+    </r>
+  </si>
+  <si>
+    <t>The propulsion system shall provide 3 Degree of Freedom motion.</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-1-2</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-2-1</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-2-2</t>
+  </si>
+  <si>
+    <t>The system used for primary spacecraft navigation shall be able to integrate into the Colony-II bus.</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-1-3</t>
+  </si>
+  <si>
+    <t>The system used for primary spacecraft navigation shall incorperate a control algorithms for realtive spacecraft navigation.</t>
+  </si>
+  <si>
+    <t>The Rascal mission shall consist of a primary spacecraft that will perform rendezvous and proximity operations realtive to a target secondary sapcecraft, or resident space object (RSO)</t>
+  </si>
+  <si>
+    <t>Both the secondary and primary spacecraft shall be physically conjoined prior to launch.</t>
+  </si>
+  <si>
+    <t>Both the seondary and primary spacecraft shall be physically conjoined during launch.</t>
+  </si>
+  <si>
+    <t>Both the secondary and primary spacecraft shall be physically conjoined during launch vehicle separation.</t>
+  </si>
+  <si>
+    <t>Both the secondary and primary spacecraft shall be physically conjoined during initial on-orbit operations.</t>
+  </si>
+  <si>
+    <t>The secondary shall operate for a period of two weeks after separation, with a goal of four weeks.</t>
+  </si>
+  <si>
+    <t>The primary spacecraft shall resolve the relative distance and angle between the secondary and primary spacecraft over a range of 0.1-100 meters, with a maximum goal of 2000 meters.</t>
+  </si>
+  <si>
+    <t>The secondary spacecraft shall provide navigation aids to the primary spacecraft, as specified in the RCL-O-ADC1 ADC Overview document.</t>
+  </si>
+  <si>
+    <t>The secondary spacecraft's navigation aids shall be able to be remotely powered on and off.</t>
+  </si>
+  <si>
+    <t>Both the secondary and primary spacecraft shall integrate into the same 6U CubeSat Deployer.</t>
+  </si>
+  <si>
+    <t>The method used to conjoin the secondary and primary spacecraft shall withstand the loads associated with the launch vehicle environment, as specified by the LSP or by the Proto-Qualification NASA GEVS Random Vibration Profile.</t>
+  </si>
+  <si>
+    <t>The method used to conjoin the secondary and primary spacecraft shall withstand the impulsive load associated with a 2 m/s launch ejection speed.</t>
+  </si>
+  <si>
+    <t>The secondary spacecraft shall physically separate from the primary spacecraft upon command from the ground.</t>
+  </si>
+  <si>
+    <t>The secondary and primary spacecraft shall separate with a relative speed no more than 1 m/s, with a  goal of 5 cm/s.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The secondary  shall separate from the primary spacecraft with a rotational rate no more than 10 </t>
     </r>
     <r>
       <rPr>
@@ -302,127 +426,6 @@
       </rPr>
       <t>/s.</t>
     </r>
-  </si>
-  <si>
-    <t>RCL-RVM1-1</t>
-  </si>
-  <si>
-    <t>RCL-RVM1-2</t>
-  </si>
-  <si>
-    <t>The RSO shall physically separate from the primary spacecraft upon command from the ground.</t>
-  </si>
-  <si>
-    <t>Both the RSO and primary spacecraft shall be physically conjoined prior to launch.</t>
-  </si>
-  <si>
-    <t>Both the RSO and primary spacecraft shall be physically conjoined during launch.</t>
-  </si>
-  <si>
-    <t>RCL-RVM5</t>
-  </si>
-  <si>
-    <t>Both the RSO and primary spacecraft shall be physically conjoined during launch vehicle separation.</t>
-  </si>
-  <si>
-    <t>RCL-RVM6</t>
-  </si>
-  <si>
-    <t>Both the RSO and primary spacecraft shall integrate into the same 6U CubeSat Deployer.</t>
-  </si>
-  <si>
-    <t>RCL-RVM2-1</t>
-  </si>
-  <si>
-    <t>RVM5 Sub-Requirements</t>
-  </si>
-  <si>
-    <t>RCL-RVM5-1</t>
-  </si>
-  <si>
-    <t>RVM5-1 Sub-Requirements</t>
-  </si>
-  <si>
-    <t>RCL-RVM5-1-1</t>
-  </si>
-  <si>
-    <t>RCL-RVM5-1-2</t>
-  </si>
-  <si>
-    <t>RVM4 Sub-Requirements</t>
-  </si>
-  <si>
-    <t>RCL-RVM4-1</t>
-  </si>
-  <si>
-    <t>Both the RSO and primary spacecraft shall be physically conjoined during initial on-orbit operations.</t>
-  </si>
-  <si>
-    <t>The method used to conjoin the RSO and primary spacecraft shall withstand the loads associated with the launch vehicle environment, as specified by the LSP or by the Proto-Qualification NASA GEVS Random Vibration Profile.</t>
-  </si>
-  <si>
-    <t>The method used to conjoin the RSO and primary spacecraft shall withstand the impulsive load associated with a 2 m/s launch ejection speed.</t>
-  </si>
-  <si>
-    <t>The primary spacecraft shall utilize a propulsion system to execute all RPO maneuvers.</t>
-  </si>
-  <si>
-    <t>The primary spacecraft shall resolve the relative distance and angle between the RSO and primary spacecraft over a range of 0.1-100 meters, with a maximum goal of 2000 meters.</t>
-  </si>
-  <si>
-    <t>RCL-RVM1-1-1</t>
-  </si>
-  <si>
-    <t>RVM1-1 Sub-Requirements</t>
-  </si>
-  <si>
-    <t>The RSO's navigation aids shall be able to be remotely powered on and off.</t>
-  </si>
-  <si>
-    <t>The RSO shall provide navigation aids to the primary spacecraft, as specified in the RCL-O-ADC1 ADC Overview document.</t>
-  </si>
-  <si>
-    <t>The RSO shall operate for a period of two weeks after separation, with a goal of four weeks.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The propulsion system shall provide a total </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Δ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.35"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>V capability of 50 m/s, with a  goal of 100 m/s</t>
-    </r>
-  </si>
-  <si>
-    <t>The propulsion system shall provide 3 Degree of Freedom motion.</t>
-  </si>
-  <si>
-    <t>RCL-RVM1-1-2</t>
-  </si>
-  <si>
-    <t>RCL-RVM1-2-1</t>
-  </si>
-  <si>
-    <t>RCL-RVM1-2-2</t>
-  </si>
-  <si>
-    <t>The system used for primary spacecraft navigation shall be able to integrate into the Colony-II bus.</t>
-  </si>
-  <si>
-    <t>RCL-RVM1-1-3</t>
   </si>
 </sst>
 </file>
@@ -2169,11 +2172,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T203"/>
+  <dimension ref="A1:T204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2232,15 +2235,15 @@
     </row>
     <row r="4" spans="1:7" ht="45">
       <c r="A4" s="46" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B4" s="47"/>
       <c r="C4" s="47"/>
       <c r="D4" s="47"/>
-      <c r="E4" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="47" t="s">
+      <c r="E4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="10" t="s">
@@ -2249,7 +2252,7 @@
     </row>
     <row r="5" spans="1:7" ht="30">
       <c r="A5" s="9" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>53</v>
@@ -2272,7 +2275,7 @@
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="9" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>53</v>
@@ -2295,7 +2298,7 @@
     </row>
     <row r="7" spans="1:7" ht="30">
       <c r="A7" s="9" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>53</v>
@@ -2318,7 +2321,7 @@
     </row>
     <row r="8" spans="1:7" ht="30">
       <c r="A8" s="9" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>53</v>
@@ -2336,12 +2339,12 @@
         <v>36</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30">
       <c r="A9" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>53</v>
@@ -2357,7 +2360,7 @@
         <v>36</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.25">
@@ -2373,7 +2376,7 @@
     </row>
     <row r="11" spans="1:7" ht="45">
       <c r="A11" s="11" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>53</v>
@@ -2389,12 +2392,12 @@
         <v>74</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30">
       <c r="A12" s="11" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -2406,12 +2409,12 @@
         <v>36</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25">
       <c r="A13" s="40" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
@@ -2422,7 +2425,7 @@
     </row>
     <row r="14" spans="1:7" ht="30">
       <c r="A14" s="11" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -2434,82 +2437,82 @@
         <v>74</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30">
       <c r="A15" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>53</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45">
       <c r="A16" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>53</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="F16" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="14.25">
-      <c r="A17" s="40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="30">
+      <c r="A17" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="14.25">
+      <c r="A18" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-    </row>
-    <row r="18" spans="1:20" ht="27">
-      <c r="A18" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="15">
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+    </row>
+    <row r="19" spans="1:20" ht="27">
       <c r="A19" s="11" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>53</v>
@@ -2521,53 +2524,44 @@
         <v>53</v>
       </c>
       <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="F19" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="G19" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A20" s="45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="15">
+      <c r="A20" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" s="12" customFormat="1" ht="15">
+      <c r="A21" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-    </row>
-    <row r="21" spans="1:20" s="12" customFormat="1" ht="30">
-      <c r="A21" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
@@ -2582,16 +2576,24 @@
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
     </row>
-    <row r="22" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A22" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
+    <row r="22" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A22" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
@@ -2606,22 +2608,16 @@
       <c r="S22" s="15"/>
       <c r="T22" s="15"/>
     </row>
-    <row r="23" spans="1:20" s="12" customFormat="1" ht="60">
-      <c r="A23" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>80</v>
-      </c>
+    <row r="23" spans="1:20" s="12" customFormat="1" ht="15">
+      <c r="A23" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
@@ -2636,16 +2632,22 @@
       <c r="S23" s="15"/>
       <c r="T23" s="15"/>
     </row>
-    <row r="24" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A24" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
+    <row r="24" spans="1:20" s="12" customFormat="1" ht="60">
+      <c r="A24" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
@@ -2660,24 +2662,16 @@
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
     </row>
-    <row r="25" spans="1:20" s="12" customFormat="1" ht="45">
-      <c r="A25" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>98</v>
-      </c>
+    <row r="25" spans="1:20" s="12" customFormat="1" ht="15">
+      <c r="A25" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
@@ -2692,16 +2686,24 @@
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
     </row>
-    <row r="26" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A26" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
+    <row r="26" spans="1:20" s="12" customFormat="1" ht="45">
+      <c r="A26" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
@@ -2716,24 +2718,16 @@
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
     </row>
-    <row r="27" spans="1:20" s="12" customFormat="1" ht="30">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:20" s="12" customFormat="1" ht="15">
+      <c r="A27" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>93</v>
-      </c>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
@@ -2748,16 +2742,24 @@
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
     </row>
-    <row r="28" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A28" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
+    <row r="28" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A28" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
@@ -2772,24 +2774,16 @@
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
     </row>
-    <row r="29" spans="1:20" s="12" customFormat="1" ht="30">
-      <c r="A29" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>95</v>
-      </c>
+    <row r="29" spans="1:20" s="12" customFormat="1" ht="15">
+      <c r="A29" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
@@ -2806,7 +2800,7 @@
     </row>
     <row r="30" spans="1:20" s="12" customFormat="1" ht="30">
       <c r="A30" s="9" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -2820,7 +2814,7 @@
         <v>36</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
@@ -2836,14 +2830,24 @@
       <c r="S30" s="15"/>
       <c r="T30" s="15"/>
     </row>
-    <row r="31" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
+    <row r="31" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A31" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>88</v>
+      </c>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
@@ -3498,6 +3502,25 @@
     </row>
     <row r="61" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A61" s="14"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="15"/>
+      <c r="S61" s="15"/>
+      <c r="T61" s="15"/>
     </row>
     <row r="62" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A62" s="14"/>
@@ -3545,7 +3568,7 @@
       <c r="A76" s="14"/>
     </row>
     <row r="77" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A77" s="13"/>
+      <c r="A77" s="14"/>
     </row>
     <row r="78" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A78" s="13"/>
@@ -3924,22 +3947,25 @@
     </row>
     <row r="203" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A203" s="13"/>
+    </row>
+    <row r="204" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A204" s="13"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
-    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A18:G18"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A27:G27"/>
     <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A25:G25"/>
     <mergeCell ref="A13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>

</xml_diff>

<commit_message>
Reordered some toplevel requirements and added propulsion requirements
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
   <si>
     <t>Document Title</t>
   </si>
@@ -265,6 +265,9 @@
     <t>RCL-RVM1-2</t>
   </si>
   <si>
+    <t>RCL-RVM1-3</t>
+  </si>
+  <si>
     <t>RCL-RVM5</t>
   </si>
   <si>
@@ -295,40 +298,12 @@
     <t>RCL-RVM4-1</t>
   </si>
   <si>
-    <t>The primary spacecraft shall utilize a propulsion system to execute all RPO maneuvers.</t>
-  </si>
-  <si>
     <t>RCL-RVM1-1-1</t>
   </si>
   <si>
     <t>RVM1-1 Sub-Requirements</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The propulsion system shall provide a total </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Δ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.35"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>V capability of 50 m/s, with a  goal of 100 m/s</t>
-    </r>
-  </si>
-  <si>
-    <t>The propulsion system shall provide 3 Degree of Freedom motion.</t>
-  </si>
-  <si>
     <t>RCL-RVM1-1-2</t>
   </si>
   <si>
@@ -338,40 +313,19 @@
     <t>RCL-RVM1-2-2</t>
   </si>
   <si>
-    <t>The system used for primary spacecraft navigation shall be able to integrate into the Colony-II bus.</t>
-  </si>
-  <si>
-    <t>RCL-RVM1-1-3</t>
-  </si>
-  <si>
-    <t>The system used for primary spacecraft navigation shall incorperate a control algorithms for realtive spacecraft navigation.</t>
-  </si>
-  <si>
-    <t>The Rascal mission shall consist of a primary spacecraft that will perform rendezvous and proximity operations realtive to a target secondary sapcecraft, or resident space object (RSO)</t>
-  </si>
-  <si>
     <t>Both the secondary and primary spacecraft shall be physically conjoined prior to launch.</t>
   </si>
   <si>
-    <t>Both the seondary and primary spacecraft shall be physically conjoined during launch.</t>
-  </si>
-  <si>
     <t>Both the secondary and primary spacecraft shall be physically conjoined during launch vehicle separation.</t>
   </si>
   <si>
     <t>Both the secondary and primary spacecraft shall be physically conjoined during initial on-orbit operations.</t>
   </si>
   <si>
-    <t>The secondary shall operate for a period of two weeks after separation, with a goal of four weeks.</t>
-  </si>
-  <si>
     <t>The primary spacecraft shall resolve the relative distance and angle between the secondary and primary spacecraft over a range of 0.1-100 meters, with a maximum goal of 2000 meters.</t>
   </si>
   <si>
     <t>The secondary spacecraft shall provide navigation aids to the primary spacecraft, as specified in the RCL-O-ADC1 ADC Overview document.</t>
-  </si>
-  <si>
-    <t>The secondary spacecraft's navigation aids shall be able to be remotely powered on and off.</t>
   </si>
   <si>
     <t>Both the secondary and primary spacecraft shall integrate into the same 6U CubeSat Deployer.</t>
@@ -427,12 +381,95 @@
       <t>/s.</t>
     </r>
   </si>
+  <si>
+    <t>Both the secondary and primary spacecraft shall be physically conjoined during launch.</t>
+  </si>
+  <si>
+    <t>The system used for primary spacecraft navigation shall incorporate a control algorithm for relative spacecraft navigation.</t>
+  </si>
+  <si>
+    <t>The Rascal mission shall consist of a primary spacecraft that will perform rendezvous and proximity operations (RPO) relative to a target secondary spacecraft.</t>
+  </si>
+  <si>
+    <t>The primary spacecraft shall perform the orbirtal maneuvers defined in the RCL-O-CMQA3 Rascal Concept of Operations document.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The primary spacecraft shall provide a total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>V capability of 50 m/s, with a  goal of 100 m/s</t>
+    </r>
+  </si>
+  <si>
+    <t>The primary sapcecraft shall provide 3 Degrees of Freedom motion, as defined by the primary axes of its local coordinate frame.</t>
+  </si>
+  <si>
+    <t>RVM1-2-2 Sub-Requirements</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The system used to provide this </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>V capability shall be constrained to a 0.5U volume.</t>
+    </r>
+  </si>
+  <si>
+    <t>RCL-RVM1-2-2-1</t>
+  </si>
+  <si>
+    <t>The mass of the system shall be no more than 75% of the payload mass, with a goal of 50%.</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-2-2-2</t>
+  </si>
+  <si>
+    <t>The system used for primary spacecraft navigation and maneuvering shall be able to integrate into the Colony-II bus.</t>
+  </si>
+  <si>
+    <t>RCL-RVM7</t>
+  </si>
+  <si>
+    <t>The primary spacecraft shall have an operational life of 6 months, with a goal of 3 years.</t>
+  </si>
+  <si>
+    <t>After separation, the secondary spacecraft shall have an operational life  of two weeks, with a goal of four weeks.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -480,20 +517,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="9"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Times New Roman"/>
@@ -515,8 +538,35 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color indexed="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,6 +607,12 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="62"/>
       </patternFill>
     </fill>
   </fills>
@@ -739,7 +795,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -784,17 +840,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -806,50 +862,44 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -857,14 +907,23 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2172,11 +2231,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T204"/>
+  <dimension ref="A1:T207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2189,24 +2248,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="43" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="40" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25">
-      <c r="A2" s="43"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="16" t="s">
         <v>49</v>
       </c>
@@ -2219,27 +2278,27 @@
       <c r="E2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="41"/>
-    </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A3" s="42" t="s">
+      <c r="F2" s="41"/>
+      <c r="G2" s="40"/>
+    </row>
+    <row r="3" spans="1:7" ht="22.5">
+      <c r="A3" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="1:7" ht="45">
-      <c r="A4" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
+      <c r="A4" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="10" t="s">
         <v>53</v>
       </c>
@@ -2252,7 +2311,7 @@
     </row>
     <row r="5" spans="1:7" ht="30">
       <c r="A5" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>53</v>
@@ -2275,7 +2334,7 @@
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="9" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>53</v>
@@ -2298,7 +2357,7 @@
     </row>
     <row r="7" spans="1:7" ht="30">
       <c r="A7" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>53</v>
@@ -2321,7 +2380,7 @@
     </row>
     <row r="8" spans="1:7" ht="30">
       <c r="A8" s="9" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>53</v>
@@ -2339,12 +2398,12 @@
         <v>36</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30">
       <c r="A9" s="9" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>53</v>
@@ -2360,127 +2419,129 @@
         <v>36</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="14.25">
-      <c r="A10" s="45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30">
+      <c r="A10" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20.25">
+      <c r="A11" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-    </row>
-    <row r="11" spans="1:7" ht="45">
-      <c r="A11" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10" t="s">
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+    </row>
+    <row r="12" spans="1:7" ht="45">
+      <c r="A12" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
-      <c r="A12" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="10" t="s">
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.25">
-      <c r="A13" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-    </row>
-    <row r="14" spans="1:7" ht="30">
+    <row r="14" spans="1:7" ht="35.25" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="F14" s="10" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30">
-      <c r="A15" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75">
+      <c r="A15" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+    </row>
+    <row r="16" spans="1:7" ht="30">
       <c r="A16" s="11" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="30">
       <c r="A17" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>53</v>
@@ -2488,31 +2549,29 @@
       <c r="C17" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="14.25">
-      <c r="A18" s="40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="18.75">
+      <c r="A18" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-    </row>
-    <row r="19" spans="1:20" ht="27">
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+    </row>
+    <row r="19" spans="1:20" ht="30">
       <c r="A19" s="11" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>53</v>
@@ -2528,12 +2587,12 @@
         <v>36</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="27">
       <c r="A20" s="11" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>53</v>
@@ -2549,42 +2608,27 @@
         <v>36</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A21" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-    </row>
-    <row r="22" spans="1:20" s="12" customFormat="1" ht="30">
-      <c r="A22" s="9" t="s">
-        <v>111</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="15.75">
+      <c r="A21" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+    </row>
+    <row r="22" spans="1:20" ht="27">
+      <c r="A22" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="D22" s="10"/>
       <c r="E22" s="10" t="s">
         <v>53</v>
       </c>
@@ -2592,62 +2636,36 @@
         <v>36</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-    </row>
-    <row r="23" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A23" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-    </row>
-    <row r="24" spans="1:20" s="12" customFormat="1" ht="60">
-      <c r="A24" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>78</v>
-      </c>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="30">
+      <c r="A23" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="12" customFormat="1" ht="20.25">
+      <c r="A24" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
@@ -2662,16 +2680,24 @@
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
     </row>
-    <row r="25" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A25" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
+    <row r="25" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>84</v>
+      </c>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
@@ -2686,24 +2712,16 @@
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
     </row>
-    <row r="26" spans="1:20" s="12" customFormat="1" ht="45">
-      <c r="A26" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>90</v>
-      </c>
+    <row r="26" spans="1:20" s="12" customFormat="1" ht="20.25">
+      <c r="A26" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
@@ -2718,16 +2736,22 @@
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
     </row>
-    <row r="27" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A27" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
+    <row r="27" spans="1:20" s="12" customFormat="1" ht="60">
+      <c r="A27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
@@ -2742,24 +2766,16 @@
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
     </row>
-    <row r="28" spans="1:20" s="12" customFormat="1" ht="30">
-      <c r="A28" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>85</v>
-      </c>
+    <row r="28" spans="1:20" s="12" customFormat="1" ht="20.25">
+      <c r="A28" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
@@ -2774,16 +2790,24 @@
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
     </row>
-    <row r="29" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A29" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
+    <row r="29" spans="1:20" s="12" customFormat="1" ht="45">
+      <c r="A29" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
@@ -2798,24 +2822,16 @@
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
     </row>
-    <row r="30" spans="1:20" s="12" customFormat="1" ht="30">
-      <c r="A30" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>87</v>
-      </c>
+    <row r="30" spans="1:20" s="12" customFormat="1" ht="20.25">
+      <c r="A30" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
@@ -2831,8 +2847,8 @@
       <c r="T30" s="15"/>
     </row>
     <row r="31" spans="1:20" s="12" customFormat="1" ht="30">
-      <c r="A31" s="9" t="s">
-        <v>116</v>
+      <c r="A31" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -2846,7 +2862,7 @@
         <v>36</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
@@ -2862,14 +2878,16 @@
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
     </row>
-    <row r="32" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
+    <row r="32" spans="1:20" s="12" customFormat="1" ht="18.75">
+      <c r="A32" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
@@ -2884,14 +2902,24 @@
       <c r="S32" s="15"/>
       <c r="T32" s="15"/>
     </row>
-    <row r="33" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A33" s="14"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
+    <row r="33" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A33" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>88</v>
+      </c>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
@@ -2906,14 +2934,24 @@
       <c r="S33" s="15"/>
       <c r="T33" s="15"/>
     </row>
-    <row r="34" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A34" s="14"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
+    <row r="34" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A34" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
@@ -3524,12 +3562,69 @@
     </row>
     <row r="62" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A62" s="14"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
+      <c r="Q62" s="15"/>
+      <c r="R62" s="15"/>
+      <c r="S62" s="15"/>
+      <c r="T62" s="15"/>
     </row>
     <row r="63" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A63" s="14"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="15"/>
+      <c r="R63" s="15"/>
+      <c r="S63" s="15"/>
+      <c r="T63" s="15"/>
     </row>
     <row r="64" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A64" s="14"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="O64" s="15"/>
+      <c r="P64" s="15"/>
+      <c r="Q64" s="15"/>
+      <c r="R64" s="15"/>
+      <c r="S64" s="15"/>
+      <c r="T64" s="15"/>
     </row>
     <row r="65" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A65" s="14"/>
@@ -3571,13 +3666,13 @@
       <c r="A77" s="14"/>
     </row>
     <row r="78" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A78" s="13"/>
+      <c r="A78" s="14"/>
     </row>
     <row r="79" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A79" s="13"/>
+      <c r="A79" s="14"/>
     </row>
     <row r="80" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A80" s="13"/>
+      <c r="A80" s="14"/>
     </row>
     <row r="81" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A81" s="13"/>
@@ -3951,22 +4046,32 @@
     <row r="204" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A204" s="13"/>
     </row>
+    <row r="205" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A205" s="13"/>
+    </row>
+    <row r="206" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A206" s="13"/>
+    </row>
+    <row r="207" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A207" s="13"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="13">
+  <mergeCells count="14">
     <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A21:G21"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A15:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished top level sub requirements at the moment
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA2 Secondary Spacecraft Requirements Verification Matrix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="145">
   <si>
     <t>Document Title</t>
   </si>
@@ -187,21 +187,18 @@
     <t>Verification Method(s)</t>
   </si>
   <si>
-    <t>Rationale</t>
-  </si>
-  <si>
     <t>Top Level Requirements</t>
   </si>
   <si>
-    <t xml:space="preserve">Task Number </t>
-  </si>
-  <si>
     <t>RVM1 Sub-Requirements</t>
   </si>
   <si>
     <t>RVM1-2 Sub-Requirements</t>
   </si>
   <si>
+    <t>The secondary spacecraft shall remain in a powered off state until separation.</t>
+  </si>
+  <si>
     <t>RVM2 Sub-Requirements</t>
   </si>
   <si>
@@ -259,45 +256,30 @@
     <t>RCL-RVM3-1</t>
   </si>
   <si>
+    <t>RCL-RVM3-2</t>
+  </si>
+  <si>
     <t>RCL-RVM1-1</t>
   </si>
   <si>
     <t>RCL-RVM1-2</t>
   </si>
   <si>
-    <t>RCL-RVM1-3</t>
+    <t>RCL-RVM3-1-1</t>
   </si>
   <si>
     <t>RCL-RVM5</t>
   </si>
   <si>
-    <t>RCL-RVM6</t>
-  </si>
-  <si>
     <t>RCL-RVM2-1</t>
   </si>
   <si>
-    <t>RVM5 Sub-Requirements</t>
-  </si>
-  <si>
-    <t>RCL-RVM5-1</t>
-  </si>
-  <si>
-    <t>RVM5-1 Sub-Requirements</t>
-  </si>
-  <si>
     <t>RCL-RVM5-1-1</t>
   </si>
   <si>
     <t>RCL-RVM5-1-2</t>
   </si>
   <si>
-    <t>RVM4 Sub-Requirements</t>
-  </si>
-  <si>
-    <t>RCL-RVM4-1</t>
-  </si>
-  <si>
     <t>RCL-RVM1-1-1</t>
   </si>
   <si>
@@ -313,18 +295,6 @@
     <t>RCL-RVM1-2-2</t>
   </si>
   <si>
-    <t>Both the secondary and primary spacecraft shall be physically conjoined prior to launch.</t>
-  </si>
-  <si>
-    <t>Both the secondary and primary spacecraft shall be physically conjoined during launch vehicle separation.</t>
-  </si>
-  <si>
-    <t>Both the secondary and primary spacecraft shall be physically conjoined during initial on-orbit operations.</t>
-  </si>
-  <si>
-    <t>The primary spacecraft shall resolve the relative distance and angle between the secondary and primary spacecraft over a range of 0.1-100 meters, with a maximum goal of 2000 meters.</t>
-  </si>
-  <si>
     <t>The secondary spacecraft shall provide navigation aids to the primary spacecraft, as specified in the RCL-O-ADC1 ADC Overview document.</t>
   </si>
   <si>
@@ -334,17 +304,141 @@
     <t>The method used to conjoin the secondary and primary spacecraft shall withstand the loads associated with the launch vehicle environment, as specified by the LSP or by the Proto-Qualification NASA GEVS Random Vibration Profile.</t>
   </si>
   <si>
-    <t>The method used to conjoin the secondary and primary spacecraft shall withstand the impulsive load associated with a 2 m/s launch ejection speed.</t>
-  </si>
-  <si>
     <t>The secondary spacecraft shall physically separate from the primary spacecraft upon command from the ground.</t>
   </si>
   <si>
     <t>The secondary and primary spacecraft shall separate with a relative speed no more than 1 m/s, with a  goal of 5 cm/s.</t>
   </si>
   <si>
+    <t>Requirement Driver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement Number </t>
+  </si>
+  <si>
+    <t>The primary spacecraft shall have an operational life of at least 6 months, with a goal of 3 years.</t>
+  </si>
+  <si>
+    <t>After separation, the secondary spacecraft shall have an operational life  of at least two weeks, with a goal of one month.</t>
+  </si>
+  <si>
+    <t>The SSRL shall provide a target resident space object (RSO) that will be used as the target object for RPO and SSA mission capabilities. This RSO will be given the designation of the Secondary Spacecraft.</t>
+  </si>
+  <si>
+    <t>The payload that is provided by the SSRL shall be integrated into Boeing's Colony-II bus. Together, these are designated as the Primary Spacecraft.</t>
+  </si>
+  <si>
+    <t>RCL-RVM3-3</t>
+  </si>
+  <si>
+    <t>RCL-RVM3-4</t>
+  </si>
+  <si>
+    <t>RVM3-2 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>RCL-RVM3-2-1</t>
+  </si>
+  <si>
+    <t>RVM3-3 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>RCL-RVM3-3-1</t>
+  </si>
+  <si>
+    <t>RCL-RVM3-5</t>
+  </si>
+  <si>
+    <t>RCL-RVM3-6</t>
+  </si>
+  <si>
+    <t>RCL-RVM3-7</t>
+  </si>
+  <si>
+    <t>RVM3-4 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>The secondary and primary spacecraft shall withstand an instantaneous impulsive load associated with at least a 2 m/s change in velocity, with a  goal of 3 m/s.</t>
+  </si>
+  <si>
+    <t>The SSRL shall provide a payload that will be used to demonstrate Rendezvous and Proximity Operations (RPO) and Space Situational Awareness (SSA) mission capabilities.</t>
+  </si>
+  <si>
+    <t>The secondary spacecraft shall conform to the 3U CubeSat Design Specification</t>
+  </si>
+  <si>
+    <t>The secondary spacecraft shall be physically conjoined to the primary spacecraft prior to launch vehicle integration.</t>
+  </si>
+  <si>
+    <t>The secondary spacecraft shall be physically conjoined to the primary spacecraft during launch.</t>
+  </si>
+  <si>
+    <t>The secondary spacecraft shall be physically conjoined to the primary spacecraft during launch vehicle separation.</t>
+  </si>
+  <si>
+    <t>RVM3-6 Sub-Requirements</t>
+  </si>
+  <si>
+    <t>The secondary spacecraft shall be physically conjoined to the primary spacecraft during initial on-orbit operations for at least 1 month, with a goal of two months.</t>
+  </si>
+  <si>
+    <t>RCL-RVM3-8</t>
+  </si>
+  <si>
+    <t>The primary spacecraft payload shall include a propulsion system for executing the RPO maneuvers outlined in the RCL-O-CMQA3 Concept of Operations document.</t>
+  </si>
+  <si>
+    <t>The primary spacecraft payload shall resolve relative position and attitude data between the secondary and primary spacecraft over a range of 0-100 meters, with a maximum goal of 2000 meters.</t>
+  </si>
+  <si>
+    <t>The total volume of the primary spacecraft payload shall be no greater than 1.5U's (10x10x15cm)</t>
+  </si>
+  <si>
+    <t>RCL-RVM2-2</t>
+  </si>
+  <si>
+    <t>RCL-RVM2-3</t>
+  </si>
+  <si>
+    <t>RCL-RVM2-4</t>
+  </si>
+  <si>
+    <t>RCL-RVM2-5</t>
+  </si>
+  <si>
+    <t>The average power draw of the primary spacecraft payload shall be no greater than 10 Watts (W).</t>
+  </si>
+  <si>
+    <t>RCL-RVM2-6</t>
+  </si>
+  <si>
+    <t>The primary spacecraft propulsion unit shall provide 3 Degrees of Freedom motion, as defined by the primary axes of its local coordinate frame.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">The secondary  shall separate from the primary spacecraft with a rotational rate no more than 10 </t>
+      <t xml:space="preserve">The primary spacecraft propulsion unit shall provide a total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>V capability of 50 m/s, with a  goal of 100 m/s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The secondary  shall separate from the primary spacecraft with a local slew rate no more than 10 </t>
     </r>
     <r>
       <rPr>
@@ -382,94 +476,47 @@
     </r>
   </si>
   <si>
-    <t>Both the secondary and primary spacecraft shall be physically conjoined during launch.</t>
-  </si>
-  <si>
-    <t>The system used for primary spacecraft navigation shall incorporate a control algorithm for relative spacecraft navigation.</t>
-  </si>
-  <si>
-    <t>The Rascal mission shall consist of a primary spacecraft that will perform rendezvous and proximity operations (RPO) relative to a target secondary spacecraft.</t>
-  </si>
-  <si>
-    <t>The primary spacecraft shall perform the orbirtal maneuvers defined in the RCL-O-CMQA3 Rascal Concept of Operations document.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The primary spacecraft shall provide a total </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Δ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.35"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>V capability of 50 m/s, with a  goal of 100 m/s</t>
-    </r>
-  </si>
-  <si>
-    <t>The primary sapcecraft shall provide 3 Degrees of Freedom motion, as defined by the primary axes of its local coordinate frame.</t>
-  </si>
-  <si>
-    <t>RVM1-2-2 Sub-Requirements</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The system used to provide this </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Δ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.35"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>V capability shall be constrained to a 0.5U volume.</t>
-    </r>
-  </si>
-  <si>
-    <t>RCL-RVM1-2-2-1</t>
-  </si>
-  <si>
-    <t>The mass of the system shall be no more than 75% of the payload mass, with a goal of 50%.</t>
-  </si>
-  <si>
-    <t>RCL-RVM1-2-2-2</t>
-  </si>
-  <si>
-    <t>The system used for primary spacecraft navigation and maneuvering shall be able to integrate into the Colony-II bus.</t>
-  </si>
-  <si>
-    <t>RCL-RVM7</t>
-  </si>
-  <si>
-    <t>The primary spacecraft shall have an operational life of 6 months, with a goal of 3 years.</t>
-  </si>
-  <si>
-    <t>After separation, the secondary spacecraft shall have an operational life  of two weeks, with a goal of four weeks.</t>
+    <t>RCL-RVM1-2-3</t>
+  </si>
+  <si>
+    <t>The primary spacecraft payload shall conform to the CubeSat Design Specifications Rev 12</t>
+  </si>
+  <si>
+    <t>The total mass of the primary spacecraft payload shall be no greater than 3 kg.</t>
+  </si>
+  <si>
+    <t>The peak power draw of the primary spacecraft payload shall not exceed 30 W.</t>
+  </si>
+  <si>
+    <t>The primary spacecraft payload will utilize the RS422 protocol for data communication between it and the Colony-II bus.</t>
+  </si>
+  <si>
+    <t>The primary spacecraft propulsion unit shall utilize cold-gas for all thrusting.</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-2-4</t>
+  </si>
+  <si>
+    <t>RCL-RVM1-2-5</t>
+  </si>
+  <si>
+    <t>The total volume of the primary spacecraft propulsion system shall not exceed 0.5U's (10x10x5cm)</t>
+  </si>
+  <si>
+    <t>The total mass of the primary spacecraft propulsion system shall be no more than 75% of the payload mass, with a goal of 50%.</t>
+  </si>
+  <si>
+    <t>The primary spacecraft payload shall provide navigation solutions for the position and attitude data produced by the payload vision system and Colony-II guidance, navigation, and control (GNC) system.</t>
+  </si>
+  <si>
+    <t>The primary spacecraft shall utilize a vision system for the resolution of relative spacecraft position and attitude data.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -559,14 +606,8 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -609,14 +650,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="62"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -789,13 +824,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -853,6 +949,12 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -898,12 +1000,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -913,18 +1009,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -1635,67 +1735,67 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="29">
         <v>41582</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
@@ -1948,16 +2048,16 @@
         <v>6</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1968,13 +2068,13 @@
         <v>41726</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2085,89 +2185,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A1" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="A1" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
+      <c r="A2" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="34"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="32"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="34"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="32"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="20"/>
@@ -2179,44 +2279,44 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
+      <c r="A11" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
     </row>
     <row r="12" spans="1:7" ht="59.25" customHeight="1">
-      <c r="A12" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
+      <c r="A12" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
     </row>
     <row r="13" spans="1:7" ht="59.25" customHeight="1">
-      <c r="A13" s="39"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
     </row>
     <row r="14" spans="1:7" ht="59.25" customHeight="1">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2231,11 +2331,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T207"/>
+  <dimension ref="A1:T218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2248,7 +2348,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="26" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -2257,15 +2357,15 @@
       <c r="C1" s="42"/>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
-      <c r="F1" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>57</v>
+      <c r="F1" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25">
-      <c r="A2" s="41"/>
+      <c r="A2" s="54"/>
       <c r="B2" s="16" t="s">
         <v>49</v>
       </c>
@@ -2278,86 +2378,88 @@
       <c r="E2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="40"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="55"/>
     </row>
     <row r="3" spans="1:7" ht="22.5">
       <c r="A3" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
+        <v>55</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="1:7" ht="45">
       <c r="A4" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+        <v>113</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>53</v>
+      </c>
       <c r="E4" s="10" t="s">
         <v>53</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G4" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45">
+      <c r="A5" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
-      <c r="A5" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="A6" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="10" t="s">
+    <row r="6" spans="1:7" ht="48.75" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="44" t="s">
         <v>53</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>53</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30">
       <c r="A7" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>53</v>
@@ -2368,19 +2470,17 @@
       <c r="D7" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30">
       <c r="A8" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>53</v>
@@ -2391,40 +2491,28 @@
       <c r="D8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:7" ht="20.25">
+      <c r="A9" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50"/>
+    </row>
+    <row r="10" spans="1:7" ht="45.75" customHeight="1">
+      <c r="A10" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30">
-      <c r="A10" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>53</v>
@@ -2437,47 +2525,43 @@
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="20.25">
-      <c r="A11" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-    </row>
-    <row r="12" spans="1:7" ht="45">
-      <c r="A12" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="10" t="s">
         <v>79</v>
       </c>
+    </row>
+    <row r="11" spans="1:7" ht="45">
+      <c r="A11" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75">
+      <c r="A12" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="53"/>
     </row>
     <row r="13" spans="1:7" ht="30">
       <c r="A13" s="11" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -2486,162 +2570,170 @@
         <v>53</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="35.25" customHeight="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60">
       <c r="A14" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+        <v>143</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="D14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75">
-      <c r="A15" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-    </row>
-    <row r="16" spans="1:7" ht="30">
+      <c r="A15" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53"/>
+    </row>
+    <row r="16" spans="1:7" ht="45">
       <c r="A16" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+        <v>130</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="D16" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="30">
       <c r="A17" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>53</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="F17" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="27">
+      <c r="A18" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="18.75">
-      <c r="A18" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
+      <c r="G18" s="10" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="19" spans="1:20" ht="30">
       <c r="A19" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="10"/>
+        <v>141</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="F19" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="27">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="30">
       <c r="A20" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="10"/>
+        <v>142</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="F20" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="20.25">
       <c r="A21" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-    </row>
-    <row r="22" spans="1:20" ht="27">
+        <v>59</v>
+      </c>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="50"/>
+    </row>
+    <row r="22" spans="1:20" ht="30">
       <c r="A22" s="11" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="E22" s="10" t="s">
         <v>53</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="30">
       <c r="A23" s="11" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -2650,132 +2742,94 @@
         <v>53</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" s="12" customFormat="1" ht="20.25">
-      <c r="A24" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-    </row>
-    <row r="25" spans="1:20" s="12" customFormat="1" ht="30">
-      <c r="A25" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>53</v>
-      </c>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="30">
+      <c r="A24" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="30">
+      <c r="A25" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
-    </row>
-    <row r="26" spans="1:20" s="12" customFormat="1" ht="20.25">
-      <c r="A26" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-    </row>
-    <row r="27" spans="1:20" s="12" customFormat="1" ht="60">
-      <c r="A27" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>53</v>
-      </c>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="30">
+      <c r="A26" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="30">
+      <c r="A27" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="10"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
+      <c r="D27" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
+        <v>129</v>
+      </c>
     </row>
     <row r="28" spans="1:20" s="12" customFormat="1" ht="20.25">
-      <c r="A28" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
+      <c r="A28" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
@@ -2790,9 +2844,9 @@
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
     </row>
-    <row r="29" spans="1:20" s="12" customFormat="1" ht="45">
-      <c r="A29" s="9" t="s">
-        <v>104</v>
+    <row r="29" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A29" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>53</v>
@@ -2801,12 +2855,14 @@
         <v>53</v>
       </c>
       <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
+      <c r="E29" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="F29" s="10" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
@@ -2822,16 +2878,28 @@
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
     </row>
-    <row r="30" spans="1:20" s="12" customFormat="1" ht="20.25">
-      <c r="A30" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
+    <row r="30" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A30" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
@@ -2847,11 +2915,15 @@
       <c r="T30" s="15"/>
     </row>
     <row r="31" spans="1:20" s="12" customFormat="1" ht="30">
-      <c r="A31" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
+      <c r="A31" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="D31" s="10" t="s">
         <v>53</v>
       </c>
@@ -2862,7 +2934,7 @@
         <v>36</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
@@ -2878,16 +2950,28 @@
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
     </row>
-    <row r="32" spans="1:20" s="12" customFormat="1" ht="18.75">
-      <c r="A32" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
+    <row r="32" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A32" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>103</v>
+      </c>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
@@ -2902,12 +2986,16 @@
       <c r="S32" s="15"/>
       <c r="T32" s="15"/>
     </row>
-    <row r="33" spans="1:20" s="12" customFormat="1" ht="30">
+    <row r="33" spans="1:20" s="12" customFormat="1" ht="45">
       <c r="A33" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+        <v>119</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="D33" s="10" t="s">
         <v>53</v>
       </c>
@@ -2918,7 +3006,7 @@
         <v>36</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
@@ -2935,8 +3023,8 @@
       <c r="T33" s="15"/>
     </row>
     <row r="34" spans="1:20" s="12" customFormat="1" ht="30">
-      <c r="A34" s="9" t="s">
-        <v>107</v>
+      <c r="A34" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -2950,7 +3038,7 @@
         <v>36</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
@@ -2966,14 +3054,22 @@
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
     </row>
-    <row r="35" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A35" s="14"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
+    <row r="35" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A35" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>110</v>
+      </c>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
@@ -2988,14 +3084,24 @@
       <c r="S35" s="15"/>
       <c r="T35" s="15"/>
     </row>
-    <row r="36" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A36" s="14"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
+    <row r="36" spans="1:20" s="12" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A36" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>120</v>
+      </c>
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
@@ -3010,14 +3116,16 @@
       <c r="S36" s="15"/>
       <c r="T36" s="15"/>
     </row>
-    <row r="37" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A37" s="14"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
+    <row r="37" spans="1:20" s="12" customFormat="1" ht="18.75">
+      <c r="A37" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="52"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="53"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
@@ -3032,14 +3140,24 @@
       <c r="S37" s="15"/>
       <c r="T37" s="15"/>
     </row>
-    <row r="38" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
+    <row r="38" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A38" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
@@ -3054,14 +3172,16 @@
       <c r="S38" s="15"/>
       <c r="T38" s="15"/>
     </row>
-    <row r="39" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A39" s="14"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
+    <row r="39" spans="1:20" s="12" customFormat="1" ht="18.75">
+      <c r="A39" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="53"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
@@ -3076,14 +3196,22 @@
       <c r="S39" s="15"/>
       <c r="T39" s="15"/>
     </row>
-    <row r="40" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A40" s="14"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
+    <row r="40" spans="1:20" s="12" customFormat="1" ht="60">
+      <c r="A40" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
@@ -3098,14 +3226,16 @@
       <c r="S40" s="15"/>
       <c r="T40" s="15"/>
     </row>
-    <row r="41" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A41" s="14"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
+    <row r="41" spans="1:20" s="12" customFormat="1" ht="18.75">
+      <c r="A41" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="53"/>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
@@ -3120,14 +3250,26 @@
       <c r="S41" s="15"/>
       <c r="T41" s="15"/>
     </row>
-    <row r="42" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A42" s="14"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
+    <row r="42" spans="1:20" s="12" customFormat="1" ht="45">
+      <c r="A42" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>107</v>
+      </c>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -3142,14 +3284,16 @@
       <c r="S42" s="15"/>
       <c r="T42" s="15"/>
     </row>
-    <row r="43" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A43" s="14"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
+    <row r="43" spans="1:20" s="12" customFormat="1" ht="18.75">
+      <c r="A43" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="53"/>
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
@@ -3164,14 +3308,24 @@
       <c r="S43" s="15"/>
       <c r="T43" s="15"/>
     </row>
-    <row r="44" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A44" s="14"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
+    <row r="44" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A44" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>84</v>
+      </c>
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
@@ -3186,14 +3340,24 @@
       <c r="S44" s="15"/>
       <c r="T44" s="15"/>
     </row>
-    <row r="45" spans="1:20" s="12" customFormat="1" ht="15">
-      <c r="A45" s="14"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
+    <row r="45" spans="1:20" s="12" customFormat="1" ht="30">
+      <c r="A45" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
@@ -3626,86 +3790,295 @@
       <c r="S64" s="15"/>
       <c r="T64" s="15"/>
     </row>
-    <row r="65" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="65" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A65" s="14"/>
-    </row>
-    <row r="66" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
+      <c r="O65" s="15"/>
+      <c r="P65" s="15"/>
+      <c r="Q65" s="15"/>
+      <c r="R65" s="15"/>
+      <c r="S65" s="15"/>
+      <c r="T65" s="15"/>
+    </row>
+    <row r="66" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A66" s="14"/>
-    </row>
-    <row r="67" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B66" s="15"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="O66" s="15"/>
+      <c r="P66" s="15"/>
+      <c r="Q66" s="15"/>
+      <c r="R66" s="15"/>
+      <c r="S66" s="15"/>
+      <c r="T66" s="15"/>
+    </row>
+    <row r="67" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A67" s="14"/>
-    </row>
-    <row r="68" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+      <c r="O67" s="15"/>
+      <c r="P67" s="15"/>
+      <c r="Q67" s="15"/>
+      <c r="R67" s="15"/>
+      <c r="S67" s="15"/>
+      <c r="T67" s="15"/>
+    </row>
+    <row r="68" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A68" s="14"/>
-    </row>
-    <row r="69" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="15"/>
+      <c r="O68" s="15"/>
+      <c r="P68" s="15"/>
+      <c r="Q68" s="15"/>
+      <c r="R68" s="15"/>
+      <c r="S68" s="15"/>
+      <c r="T68" s="15"/>
+    </row>
+    <row r="69" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A69" s="14"/>
-    </row>
-    <row r="70" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B69" s="15"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="15"/>
+      <c r="P69" s="15"/>
+      <c r="Q69" s="15"/>
+      <c r="R69" s="15"/>
+      <c r="S69" s="15"/>
+      <c r="T69" s="15"/>
+    </row>
+    <row r="70" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A70" s="14"/>
-    </row>
-    <row r="71" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B70" s="15"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="15"/>
+      <c r="R70" s="15"/>
+      <c r="S70" s="15"/>
+      <c r="T70" s="15"/>
+    </row>
+    <row r="71" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A71" s="14"/>
-    </row>
-    <row r="72" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
+      <c r="S71" s="15"/>
+      <c r="T71" s="15"/>
+    </row>
+    <row r="72" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A72" s="14"/>
-    </row>
-    <row r="73" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+      <c r="T72" s="15"/>
+    </row>
+    <row r="73" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A73" s="14"/>
-    </row>
-    <row r="74" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
+      <c r="S73" s="15"/>
+      <c r="T73" s="15"/>
+    </row>
+    <row r="74" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A74" s="14"/>
-    </row>
-    <row r="75" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="15"/>
+      <c r="P74" s="15"/>
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15"/>
+      <c r="S74" s="15"/>
+      <c r="T74" s="15"/>
+    </row>
+    <row r="75" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A75" s="14"/>
-    </row>
-    <row r="76" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
+      <c r="S75" s="15"/>
+      <c r="T75" s="15"/>
+    </row>
+    <row r="76" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A76" s="14"/>
     </row>
-    <row r="77" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="77" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A77" s="14"/>
     </row>
-    <row r="78" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="78" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A78" s="14"/>
     </row>
-    <row r="79" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="79" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A79" s="14"/>
     </row>
-    <row r="80" spans="1:1" s="12" customFormat="1" ht="15">
+    <row r="80" spans="1:20" s="12" customFormat="1" ht="15">
       <c r="A80" s="14"/>
     </row>
     <row r="81" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A81" s="13"/>
+      <c r="A81" s="14"/>
     </row>
     <row r="82" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A82" s="13"/>
+      <c r="A82" s="14"/>
     </row>
     <row r="83" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A83" s="13"/>
+      <c r="A83" s="14"/>
     </row>
     <row r="84" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A84" s="13"/>
+      <c r="A84" s="14"/>
     </row>
     <row r="85" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A85" s="13"/>
+      <c r="A85" s="14"/>
     </row>
     <row r="86" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A86" s="13"/>
+      <c r="A86" s="14"/>
     </row>
     <row r="87" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A87" s="13"/>
+      <c r="A87" s="14"/>
     </row>
     <row r="88" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A88" s="13"/>
+      <c r="A88" s="14"/>
     </row>
     <row r="89" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A89" s="13"/>
+      <c r="A89" s="14"/>
     </row>
     <row r="90" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A90" s="13"/>
+      <c r="A90" s="14"/>
     </row>
     <row r="91" spans="1:1" s="12" customFormat="1" ht="15">
-      <c r="A91" s="13"/>
+      <c r="A91" s="14"/>
     </row>
     <row r="92" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A92" s="13"/>
@@ -4055,23 +4428,43 @@
     <row r="207" spans="1:1" s="12" customFormat="1" ht="15">
       <c r="A207" s="13"/>
     </row>
+    <row r="208" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A208" s="13"/>
+    </row>
+    <row r="209" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A209" s="13"/>
+    </row>
+    <row r="210" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A210" s="13"/>
+    </row>
+    <row r="211" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A211" s="13"/>
+    </row>
+    <row r="212" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A212" s="13"/>
+    </row>
+    <row r="213" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A213" s="13"/>
+    </row>
+    <row r="214" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A214" s="13"/>
+    </row>
+    <row r="215" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A215" s="13"/>
+    </row>
+    <row r="216" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A216" s="13"/>
+    </row>
+    <row r="217" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A217" s="13"/>
+    </row>
+    <row r="218" spans="1:1" s="12" customFormat="1" ht="15">
+      <c r="A218" s="13"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="14">
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A1:A2"/>
+  <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A15:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>